<commit_message>
updates to od district summary for new districts
also put the topsheet summary back in because it's working
after a fix to the inputs
</commit_message>
<xml_diff>
--- a/inputs/summary_spreadsheets/Trips_ODDistrict.xlsx
+++ b/inputs/summary_spreadsheets/Trips_ODDistrict.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="525" windowWidth="18195" windowHeight="9375"/>
+    <workbookView xWindow="-75" yWindow="4575" windowWidth="18195" windowHeight="9375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="38">
   <si>
     <t>Seattle CBD</t>
   </si>
@@ -128,11 +128,24 @@
   <si>
     <t>Scaled Survey</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Model 2010--NewDistricts</t>
+  </si>
+  <si>
+    <t>S. Kitsap</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,7 +646,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -678,8 +691,9 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -710,8 +724,13 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="20" fillId="0" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="10" xfId="44" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -739,6 +758,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -3074,10 +3094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:K42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,7 +3683,7 @@
       <c r="K16" s="12"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="1:12" ht="39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>10</v>
       </c>
@@ -3701,546 +3721,546 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B18">
-        <f>B5*$L$43/$L$15</f>
-        <v>1006675.5573147888</v>
+        <f>B5*$L$57/$L$15</f>
+        <v>1001379.7669775959</v>
       </c>
       <c r="C18">
-        <f t="shared" ref="C18:L18" si="0">C5*$L$43/$L$15</f>
-        <v>206013.25353404501</v>
+        <f t="shared" ref="C18:L18" si="0">C5*$L$57/$L$15</f>
+        <v>204929.48529365042</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>29095.841830492162</v>
+        <v>28942.778137926281</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>13974.131893284823</v>
+        <v>13900.618563082868</v>
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>5080.9199504067201</v>
+        <v>5054.1908949708368</v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>100826.98254236094</v>
+        <v>100296.56481641511</v>
       </c>
       <c r="H18">
         <f t="shared" si="0"/>
-        <v>2974.3476133711447</v>
+        <v>2958.7005449230342</v>
       </c>
       <c r="I18">
         <f t="shared" si="0"/>
-        <v>538.01956648000703</v>
+        <v>535.18922178684124</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>1439.8241626247693</v>
+        <v>1432.2497193671775</v>
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>1801.178526588868</v>
+        <v>1791.7031163960221</v>
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>1368420.0569344433</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1361221.2472861144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:L19" si="1">B6*$L$43/$L$15</f>
-        <v>204944.34067098011</v>
+        <f t="shared" ref="B19:L19" si="1">B6*$L$57/$L$15</f>
+        <v>203866.19563100036</v>
       </c>
       <c r="C19">
         <f t="shared" si="1"/>
-        <v>886024.18961327744</v>
+        <v>881363.10659822018</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>86251.426615370452</v>
+        <v>85797.686114451586</v>
       </c>
       <c r="E19">
         <f t="shared" si="1"/>
-        <v>22527.451145487579</v>
+        <v>22408.941604622112</v>
       </c>
       <c r="F19">
         <f t="shared" si="1"/>
-        <v>7652.8819055146141</v>
+        <v>7612.6226007640262</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
-        <v>44860.78048933635</v>
+        <v>44624.782618812831</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>6363.3032665116834</v>
+        <v>6329.8280125367983</v>
       </c>
       <c r="I19">
         <f t="shared" si="1"/>
-        <v>3011.6914773175968</v>
+        <v>2995.8479550344805</v>
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>4903.9094828765137</v>
+        <v>4878.1116215246793</v>
       </c>
       <c r="K19">
         <f t="shared" si="1"/>
-        <v>325.04629506053976</v>
+        <v>323.33633298187993</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>1266865.0209617326</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1260200.4590899488</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:L20" si="2">B7*$L$43/$L$15</f>
-        <v>32670.605303727221</v>
+        <f t="shared" ref="B20:L20" si="2">B7*$L$57/$L$15</f>
+        <v>32498.735951560535</v>
       </c>
       <c r="C20">
         <f t="shared" si="2"/>
-        <v>88103.151940052529</v>
+        <v>87639.670118794311</v>
       </c>
       <c r="D20">
         <f t="shared" si="2"/>
-        <v>1332735.3294876965</v>
+        <v>1325724.2455007534</v>
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>185584.97224368647</v>
+        <v>184608.67049920195</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>51263.416346276841</v>
+        <v>50993.73630590488</v>
       </c>
       <c r="G20">
         <f t="shared" si="2"/>
-        <v>66653.770085809039</v>
+        <v>66303.126436032282</v>
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>30025.226195979038</v>
+        <v>29867.273316716888</v>
       </c>
       <c r="I20">
         <f t="shared" si="2"/>
-        <v>2182.8344733936779</v>
+        <v>2171.351296288708</v>
       </c>
       <c r="J20">
         <f t="shared" si="2"/>
-        <v>3836.0876572567872</v>
+        <v>3815.9072567292183</v>
       </c>
       <c r="K20">
         <f t="shared" si="2"/>
-        <v>1728.9767067989076</v>
+        <v>1719.8811267278854</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
-        <v>1794784.3704406768</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1785342.5978087098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:L21" si="3">B8*$L$43/$L$15</f>
-        <v>15157.43796088688</v>
+        <f t="shared" ref="B21:L21" si="3">B8*$L$57/$L$15</f>
+        <v>15077.699645094272</v>
       </c>
       <c r="C21">
         <f t="shared" si="3"/>
-        <v>20988.384007153043</v>
+        <v>20877.970994330062</v>
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>188975.91662330934</v>
+        <v>187981.77623125949</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>590134.93115436402</v>
+        <v>587030.42459975614</v>
       </c>
       <c r="F21">
         <f t="shared" si="3"/>
-        <v>98062.155550266281</v>
+        <v>97546.282673415422</v>
       </c>
       <c r="G21">
         <f t="shared" si="3"/>
-        <v>92058.949883066642</v>
+        <v>91574.65790468255</v>
       </c>
       <c r="H21">
         <f t="shared" si="3"/>
-        <v>37538.662467519047</v>
+        <v>37341.183861306621</v>
       </c>
       <c r="I21">
         <f t="shared" si="3"/>
-        <v>5384.1178753624936</v>
+        <v>5355.7937949659172</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>9029.9092673388968</v>
+        <v>8982.4058727285592</v>
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>4899.4348482912137</v>
+        <v>4873.6605265261196</v>
       </c>
       <c r="L21">
         <f t="shared" si="3"/>
-        <v>1062229.8996375578</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1056641.8561040652</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:L22" si="4">B9*$L$43/$L$15</f>
-        <v>6607.1294196088038</v>
+        <f t="shared" ref="B22:L22" si="4">B9*$L$57/$L$15</f>
+        <v>6572.3714761157871</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>6931.5680482441794</v>
+        <v>6895.1033394065053</v>
       </c>
       <c r="D22">
         <f t="shared" si="4"/>
-        <v>54596.135233888555</v>
+        <v>54308.922851191055</v>
       </c>
       <c r="E22">
         <f t="shared" si="4"/>
-        <v>94457.644043399327</v>
+        <v>93960.733320809246</v>
       </c>
       <c r="F22">
         <f t="shared" si="4"/>
-        <v>567074.05937238701</v>
+        <v>564090.86850987351</v>
       </c>
       <c r="G22">
         <f t="shared" si="4"/>
-        <v>34494.308919848874</v>
+        <v>34312.84566037215</v>
       </c>
       <c r="H22">
         <f t="shared" si="4"/>
-        <v>103009.6236673466</v>
+        <v>102467.72378143843</v>
       </c>
       <c r="I22">
         <f t="shared" si="4"/>
-        <v>6900.5356287590921</v>
+        <v>6864.2341713146334</v>
       </c>
       <c r="J22">
         <f t="shared" si="4"/>
-        <v>2503.7099670815005</v>
+        <v>2490.5387691176084</v>
       </c>
       <c r="K22">
         <f t="shared" si="4"/>
-        <v>8898.7223725062959</v>
+        <v>8851.9091091750724</v>
       </c>
       <c r="L22">
         <f t="shared" si="4"/>
-        <v>885473.4366730703</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>880815.25098881405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:L23" si="5">B10*$L$43/$L$15</f>
-        <v>97939.517417187701</v>
+        <f t="shared" ref="B23:L23" si="5">B10*$L$57/$L$15</f>
+        <v>97424.289699380795</v>
       </c>
       <c r="C23">
         <f t="shared" si="5"/>
-        <v>43371.66629327042</v>
+        <v>43143.502164723846</v>
       </c>
       <c r="D23">
         <f t="shared" si="5"/>
-        <v>70127.509015860545</v>
+        <v>69758.591163510733</v>
       </c>
       <c r="E23">
         <f t="shared" si="5"/>
-        <v>97385.325637437985</v>
+        <v>96873.013341040511</v>
       </c>
       <c r="F23">
         <f t="shared" si="5"/>
-        <v>36223.796618868946</v>
+        <v>36033.235091158516</v>
       </c>
       <c r="G23">
         <f t="shared" si="5"/>
-        <v>2229763.0460536443</v>
+        <v>2218032.9931009146</v>
       </c>
       <c r="H23">
         <f t="shared" si="5"/>
-        <v>99973.680775424727</v>
+        <v>99447.751990547549</v>
       </c>
       <c r="I23">
         <f t="shared" si="5"/>
-        <v>5090.6426132093466</v>
+        <v>5063.8624100294392</v>
       </c>
       <c r="J23">
         <f t="shared" si="5"/>
-        <v>2482.2759149938915</v>
+        <v>2469.2174745566003</v>
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>6529.9143518112387</v>
+        <v>6495.5626114955576</v>
       </c>
       <c r="L23">
         <f t="shared" si="5"/>
-        <v>2688887.3746917089</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2674742.0190473585</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:L24" si="6">B11*$L$43/$L$15</f>
-        <v>3712.9799637587571</v>
+        <f t="shared" ref="B24:L24" si="6">B11*$L$57/$L$15</f>
+        <v>3693.4471924786885</v>
       </c>
       <c r="C24">
         <f t="shared" si="6"/>
-        <v>5802.0128380680035</v>
+        <v>5771.4903491679352</v>
       </c>
       <c r="D24">
         <f t="shared" si="6"/>
-        <v>24718.102418804956</v>
+        <v>24588.068579210772</v>
       </c>
       <c r="E24">
         <f t="shared" si="6"/>
-        <v>38829.290712165443</v>
+        <v>38625.02253354586</v>
       </c>
       <c r="F24">
         <f t="shared" si="6"/>
-        <v>103512.57811897452</v>
+        <v>102968.03235445569</v>
       </c>
       <c r="G24">
         <f t="shared" si="6"/>
-        <v>104623.18518516606</v>
+        <v>104072.79688068802</v>
       </c>
       <c r="H24">
         <f t="shared" si="6"/>
-        <v>1464075.8120092577</v>
+        <v>1456373.7887686833</v>
       </c>
       <c r="I24">
         <f t="shared" si="6"/>
-        <v>60710.833879505226</v>
+        <v>60391.45407030471</v>
       </c>
       <c r="J24">
         <f t="shared" si="6"/>
-        <v>3308.3984200045716</v>
+        <v>3290.9940196921416</v>
       </c>
       <c r="K24">
         <f t="shared" si="6"/>
-        <v>99070.508929823351</v>
+        <v>98549.331436162101</v>
       </c>
       <c r="L24">
         <f t="shared" si="6"/>
-        <v>1908363.7024755289</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1898324.4261843897</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:L25" si="7">B12*$L$43/$L$15</f>
-        <v>1214.0760856762827</v>
+        <f t="shared" ref="B25:L25" si="7">B12*$L$57/$L$15</f>
+        <v>1207.6892291002755</v>
       </c>
       <c r="C25">
         <f t="shared" si="7"/>
-        <v>2162.9472085701236</v>
+        <v>2151.5686518506595</v>
       </c>
       <c r="D25">
         <f t="shared" si="7"/>
-        <v>3199.1565694807409</v>
+        <v>3182.3268547581392</v>
       </c>
       <c r="E25">
         <f t="shared" si="7"/>
-        <v>5104.5913197869786</v>
+        <v>5077.7377370311251</v>
       </c>
       <c r="F25">
         <f t="shared" si="7"/>
-        <v>6183.5859212693822</v>
+        <v>6151.0561013754623</v>
       </c>
       <c r="G25">
         <f t="shared" si="7"/>
-        <v>3672.293934473902</v>
+        <v>3652.9751990658483</v>
       </c>
       <c r="H25">
         <f t="shared" si="7"/>
-        <v>58974.371827196344</v>
+        <v>58664.126976017513</v>
       </c>
       <c r="I25">
         <f t="shared" si="7"/>
-        <v>691785.09454381384</v>
+        <v>688145.83977848361</v>
       </c>
       <c r="J25">
         <f t="shared" si="7"/>
-        <v>8834.4478374446117</v>
+        <v>8787.9727013871016</v>
       </c>
       <c r="K25">
         <f t="shared" si="7"/>
-        <v>206425.05802189829</v>
+        <v>205339.12341299327</v>
       </c>
       <c r="L25">
         <f t="shared" si="7"/>
-        <v>987555.62326961046</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>982360.41664206295</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:L26" si="8">B13*$L$43/$L$15</f>
-        <v>1516.8596926148989</v>
+        <f t="shared" ref="B26:L26" si="8">B13*$L$57/$L$15</f>
+        <v>1508.8799906695622</v>
       </c>
       <c r="C26">
         <f t="shared" si="8"/>
-        <v>4560.4122254518988</v>
+        <v>4536.4213906474997</v>
       </c>
       <c r="D26">
         <f t="shared" si="8"/>
-        <v>3371.3885692130657</v>
+        <v>3353.6527983601541</v>
       </c>
       <c r="E26">
         <f t="shared" si="8"/>
-        <v>8622.6898988754729</v>
+        <v>8577.3287519644655</v>
       </c>
       <c r="F26">
         <f t="shared" si="8"/>
-        <v>1964.7374691620312</v>
+        <v>1954.4016289514441</v>
       </c>
       <c r="G26">
         <f t="shared" si="8"/>
-        <v>2190.0297962916443</v>
+        <v>2178.508766949974</v>
       </c>
       <c r="H26">
         <f t="shared" si="8"/>
-        <v>3371.7062130262193</v>
+        <v>3353.968771153262</v>
       </c>
       <c r="I26">
         <f t="shared" si="8"/>
-        <v>8168.459246065263</v>
+        <v>8125.4876578204303</v>
       </c>
       <c r="J26">
         <f t="shared" si="8"/>
-        <v>876685.83439276542</v>
+        <v>872073.87740543648</v>
       </c>
       <c r="K26">
         <f t="shared" si="8"/>
-        <v>24181.325806376422</v>
+        <v>24054.115772701312</v>
       </c>
       <c r="L26">
         <f t="shared" si="8"/>
-        <v>934633.44330984238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>929716.64293465449</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:L27" si="9">B14*$L$43/$L$15</f>
-        <v>1565.624923234323</v>
+        <f t="shared" ref="B27:L27" si="9">B14*$L$57/$L$15</f>
+        <v>1557.3886833853601</v>
       </c>
       <c r="C27">
         <f t="shared" si="9"/>
-        <v>257.12576144787255</v>
+        <v>255.77310704693406</v>
       </c>
       <c r="D27">
         <f t="shared" si="9"/>
-        <v>2091.5187824121908</v>
+        <v>2080.5159872440026</v>
       </c>
       <c r="E27">
         <f t="shared" si="9"/>
-        <v>5166.7804541623018</v>
+        <v>5139.599714742606</v>
       </c>
       <c r="F27">
         <f t="shared" si="9"/>
-        <v>6535.6595616491559</v>
+        <v>6501.2775976665507</v>
       </c>
       <c r="G27">
         <f t="shared" si="9"/>
-        <v>7017.6909534106289</v>
+        <v>6980.7731801812761</v>
       </c>
       <c r="H27">
         <f t="shared" si="9"/>
-        <v>103983.60246208019</v>
+        <v>103436.57879279186</v>
       </c>
       <c r="I27">
         <f t="shared" si="9"/>
-        <v>201323.10452682056</v>
+        <v>200264.0096239397</v>
       </c>
       <c r="J27">
         <f t="shared" si="9"/>
-        <v>24623.016433867338</v>
+        <v>24493.482810491358</v>
       </c>
       <c r="K27">
         <f t="shared" si="9"/>
-        <v>1441880.947746743</v>
+        <v>1434295.6844163926</v>
       </c>
       <c r="L27">
         <f t="shared" si="9"/>
-        <v>1794445.0716058274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>1785005.083913882</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>11</v>
       </c>
       <c r="B28">
-        <f t="shared" ref="B28:L28" si="10">B15*$L$43/$L$15</f>
-        <v>1372004.1287524637</v>
+        <f t="shared" ref="B28:L28" si="10">B15*$L$57/$L$15</f>
+        <v>1364786.4644763814</v>
       </c>
       <c r="C28">
         <f t="shared" si="10"/>
-        <v>1264214.7114695807</v>
+        <v>1257564.0920078384</v>
       </c>
       <c r="D28">
         <f t="shared" si="10"/>
-        <v>1795162.3251465282</v>
+        <v>1785718.5642186652</v>
       </c>
       <c r="E28">
         <f t="shared" si="10"/>
-        <v>1061787.8085026506</v>
+        <v>1056202.090665797</v>
       </c>
       <c r="F28">
         <f t="shared" si="10"/>
-        <v>883553.79081477551</v>
+        <v>878905.70375853637</v>
       </c>
       <c r="G28">
         <f t="shared" si="10"/>
-        <v>2686161.0378434081</v>
+        <v>2672030.0245641144</v>
       </c>
       <c r="H28">
         <f t="shared" si="10"/>
-        <v>1910290.3364977126</v>
+        <v>1900240.9248161151</v>
       </c>
       <c r="I28">
         <f t="shared" si="10"/>
-        <v>985095.33383072715</v>
+        <v>979913.06997996848</v>
       </c>
       <c r="J28">
         <f t="shared" si="10"/>
-        <v>937647.4135362542</v>
+        <v>932714.75765103078</v>
       </c>
       <c r="K28">
         <f t="shared" si="10"/>
-        <v>1795741.1136058983</v>
+        <v>1786294.3078615521</v>
       </c>
       <c r="L28">
         <f t="shared" si="10"/>
-        <v>14691658</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>14614370</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -4254,512 +4274,583 @@
       <c r="K29" s="12"/>
       <c r="L29" s="13"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="13"/>
-    </row>
-    <row r="31" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
-      <c r="L31" s="14"/>
-    </row>
-    <row r="32" spans="1:12" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="22"/>
+    </row>
+    <row r="31" spans="1:13" ht="39" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="10" t="s">
+      <c r="C31" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F31" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G31" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="H31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I31" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J32" s="10" t="s">
+      <c r="J31" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K32" s="10" t="s">
+      <c r="K31" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L32" s="10" t="s">
+      <c r="L31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="M31" s="23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="9" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B33">
-        <v>1211516</v>
-      </c>
-      <c r="C33">
-        <v>203128</v>
-      </c>
-      <c r="D33">
-        <v>36661</v>
-      </c>
-      <c r="E33">
-        <v>7244</v>
-      </c>
-      <c r="F33">
-        <v>5799</v>
-      </c>
-      <c r="G33">
-        <v>116156</v>
-      </c>
-      <c r="H33">
-        <v>8247</v>
-      </c>
-      <c r="I33">
-        <v>826</v>
-      </c>
-      <c r="J33">
-        <v>178</v>
-      </c>
-      <c r="K33">
-        <v>1781</v>
-      </c>
-      <c r="L33" s="9">
-        <f>SUM(B33:K33)</f>
-        <v>1591536</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="B32" s="22">
+        <v>1153569</v>
+      </c>
+      <c r="C32" s="22">
+        <v>212873</v>
+      </c>
+      <c r="D32" s="22">
+        <v>37119</v>
+      </c>
+      <c r="E32" s="22">
+        <v>9453</v>
+      </c>
+      <c r="F32" s="22">
+        <v>6572</v>
+      </c>
+      <c r="G32" s="22">
+        <v>114203</v>
+      </c>
+      <c r="H32" s="22">
+        <v>10462</v>
+      </c>
+      <c r="I32" s="22">
+        <v>785</v>
+      </c>
+      <c r="J32" s="22">
+        <v>315</v>
+      </c>
+      <c r="K32" s="22">
+        <v>1249</v>
+      </c>
+      <c r="L32" s="22">
+        <v>183</v>
+      </c>
+      <c r="M32" s="22">
+        <f>SUM(B32:L32)</f>
+        <v>1546783</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B34">
-        <v>202838</v>
-      </c>
-      <c r="C34">
-        <v>760268</v>
-      </c>
-      <c r="D34">
-        <v>95909</v>
-      </c>
-      <c r="E34">
-        <v>14439</v>
-      </c>
-      <c r="F34">
-        <v>8240</v>
-      </c>
-      <c r="G34">
-        <v>50392</v>
-      </c>
-      <c r="H34">
-        <v>7540</v>
-      </c>
-      <c r="I34">
-        <v>913</v>
-      </c>
-      <c r="J34">
-        <v>646</v>
-      </c>
-      <c r="K34">
-        <v>1688</v>
-      </c>
-      <c r="L34" s="9">
-        <f t="shared" ref="L34:L42" si="11">SUM(B34:K34)</f>
-        <v>1142873</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+      <c r="B33" s="22">
+        <v>212810</v>
+      </c>
+      <c r="C33" s="22">
+        <v>768330</v>
+      </c>
+      <c r="D33" s="22">
+        <v>93521</v>
+      </c>
+      <c r="E33" s="22">
+        <v>17006</v>
+      </c>
+      <c r="F33" s="22">
+        <v>9663</v>
+      </c>
+      <c r="G33" s="22">
+        <v>50295</v>
+      </c>
+      <c r="H33" s="22">
+        <v>9162</v>
+      </c>
+      <c r="I33" s="22">
+        <v>1042</v>
+      </c>
+      <c r="J33" s="22">
+        <v>1098</v>
+      </c>
+      <c r="K33" s="22">
+        <v>1440</v>
+      </c>
+      <c r="L33" s="22">
+        <v>370</v>
+      </c>
+      <c r="M33" s="22">
+        <f t="shared" ref="M33:M42" si="11">SUM(B33:L33)</f>
+        <v>1164737</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B35">
-        <v>36903</v>
-      </c>
-      <c r="C35">
-        <v>95638</v>
-      </c>
-      <c r="D35">
-        <v>933342</v>
-      </c>
-      <c r="E35">
-        <v>128525</v>
-      </c>
-      <c r="F35">
-        <v>36808</v>
-      </c>
-      <c r="G35">
-        <v>76482</v>
-      </c>
-      <c r="H35">
-        <v>21516</v>
-      </c>
-      <c r="I35">
-        <v>2031</v>
-      </c>
-      <c r="J35">
-        <v>677</v>
-      </c>
-      <c r="K35">
-        <v>3310</v>
-      </c>
-      <c r="L35" s="9">
+      <c r="B34" s="22">
+        <v>37404</v>
+      </c>
+      <c r="C34" s="22">
+        <v>93511</v>
+      </c>
+      <c r="D34" s="22">
+        <v>875899</v>
+      </c>
+      <c r="E34" s="22">
+        <v>137499</v>
+      </c>
+      <c r="F34" s="22">
+        <v>43532</v>
+      </c>
+      <c r="G34" s="22">
+        <v>78510</v>
+      </c>
+      <c r="H34" s="22">
+        <v>25960</v>
+      </c>
+      <c r="I34" s="22">
+        <v>2264</v>
+      </c>
+      <c r="J34" s="22">
+        <v>840</v>
+      </c>
+      <c r="K34" s="22">
+        <v>2855</v>
+      </c>
+      <c r="L34" s="22">
+        <v>597</v>
+      </c>
+      <c r="M34" s="22">
         <f t="shared" si="11"/>
-        <v>1335232</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+        <v>1298871</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B36">
-        <v>7230</v>
-      </c>
-      <c r="C36">
-        <v>14348</v>
-      </c>
-      <c r="D36">
-        <v>129041</v>
-      </c>
-      <c r="E36">
-        <v>443686</v>
-      </c>
-      <c r="F36">
-        <v>85711</v>
-      </c>
-      <c r="G36">
-        <v>65392</v>
-      </c>
-      <c r="H36">
-        <v>30714</v>
-      </c>
-      <c r="I36">
-        <v>2485</v>
-      </c>
-      <c r="J36">
-        <v>1645</v>
-      </c>
-      <c r="K36">
-        <v>3106</v>
-      </c>
-      <c r="L36" s="9">
+      <c r="B35" s="22">
+        <v>9377</v>
+      </c>
+      <c r="C35" s="22">
+        <v>16952</v>
+      </c>
+      <c r="D35" s="22">
+        <v>137988</v>
+      </c>
+      <c r="E35" s="22">
+        <v>415994</v>
+      </c>
+      <c r="F35" s="22">
+        <v>90876</v>
+      </c>
+      <c r="G35" s="22">
+        <v>63967</v>
+      </c>
+      <c r="H35" s="22">
+        <v>36004</v>
+      </c>
+      <c r="I35" s="22">
+        <v>2990</v>
+      </c>
+      <c r="J35" s="22">
+        <v>2112</v>
+      </c>
+      <c r="K35" s="22">
+        <v>3809</v>
+      </c>
+      <c r="L35" s="22">
+        <v>704</v>
+      </c>
+      <c r="M35" s="22">
         <f t="shared" si="11"/>
-        <v>783358</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+        <v>780773</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B37">
-        <v>5713</v>
-      </c>
-      <c r="C37">
-        <v>8096</v>
-      </c>
-      <c r="D37">
-        <v>36527</v>
-      </c>
-      <c r="E37">
-        <v>85456</v>
-      </c>
-      <c r="F37">
-        <v>602919</v>
-      </c>
-      <c r="G37">
-        <v>63943</v>
-      </c>
-      <c r="H37">
-        <v>156582</v>
-      </c>
-      <c r="I37">
-        <v>6371</v>
-      </c>
-      <c r="J37">
-        <v>2513</v>
-      </c>
-      <c r="K37">
-        <v>8969</v>
-      </c>
-      <c r="L37" s="9">
+      <c r="B36" s="22">
+        <v>6539</v>
+      </c>
+      <c r="C36" s="22">
+        <v>9562</v>
+      </c>
+      <c r="D36" s="22">
+        <v>43396</v>
+      </c>
+      <c r="E36" s="22">
+        <v>90610</v>
+      </c>
+      <c r="F36" s="22">
+        <v>583726</v>
+      </c>
+      <c r="G36" s="22">
+        <v>64524</v>
+      </c>
+      <c r="H36" s="22">
+        <v>166352</v>
+      </c>
+      <c r="I36" s="22">
+        <v>7394</v>
+      </c>
+      <c r="J36" s="22">
+        <v>1639</v>
+      </c>
+      <c r="K36" s="22">
+        <v>9047</v>
+      </c>
+      <c r="L36" s="22">
+        <v>1947</v>
+      </c>
+      <c r="M36" s="22">
         <f t="shared" si="11"/>
-        <v>977089</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+        <v>984736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B38">
-        <v>116408</v>
-      </c>
-      <c r="C38">
-        <v>50412</v>
-      </c>
-      <c r="D38">
-        <v>76296</v>
-      </c>
-      <c r="E38">
-        <v>65697</v>
-      </c>
-      <c r="F38">
-        <v>63346</v>
-      </c>
-      <c r="G38">
-        <v>2034401</v>
-      </c>
-      <c r="H38">
-        <v>140345</v>
-      </c>
-      <c r="I38">
-        <v>5461</v>
-      </c>
-      <c r="J38">
-        <v>1525</v>
-      </c>
-      <c r="K38">
-        <v>11616</v>
-      </c>
-      <c r="L38" s="9">
+      <c r="B37" s="22">
+        <v>114301</v>
+      </c>
+      <c r="C37" s="22">
+        <v>50347</v>
+      </c>
+      <c r="D37" s="22">
+        <v>78570</v>
+      </c>
+      <c r="E37" s="22">
+        <v>64206</v>
+      </c>
+      <c r="F37" s="22">
+        <v>64111</v>
+      </c>
+      <c r="G37" s="22">
+        <v>2040675</v>
+      </c>
+      <c r="H37" s="22">
+        <v>146404</v>
+      </c>
+      <c r="I37" s="22">
+        <v>5525</v>
+      </c>
+      <c r="J37" s="22">
+        <v>885</v>
+      </c>
+      <c r="K37" s="22">
+        <v>10054</v>
+      </c>
+      <c r="L37" s="22">
+        <v>1753</v>
+      </c>
+      <c r="M37" s="22">
         <f t="shared" si="11"/>
-        <v>2565507</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+        <v>2576831</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B39">
-        <v>8182</v>
-      </c>
-      <c r="C39">
-        <v>7592</v>
-      </c>
-      <c r="D39">
-        <v>21408</v>
-      </c>
-      <c r="E39">
-        <v>30997</v>
-      </c>
-      <c r="F39">
-        <v>156207</v>
-      </c>
-      <c r="G39">
-        <v>140250</v>
-      </c>
-      <c r="H39">
-        <v>1860632</v>
-      </c>
-      <c r="I39">
-        <v>70753</v>
-      </c>
-      <c r="J39">
-        <v>3329</v>
-      </c>
-      <c r="K39">
-        <v>120887</v>
-      </c>
-      <c r="L39" s="9">
+      <c r="B38" s="22">
+        <v>10359</v>
+      </c>
+      <c r="C38" s="22">
+        <v>9100</v>
+      </c>
+      <c r="D38" s="22">
+        <v>25817</v>
+      </c>
+      <c r="E38" s="22">
+        <v>36294</v>
+      </c>
+      <c r="F38" s="22">
+        <v>166061</v>
+      </c>
+      <c r="G38" s="22">
+        <v>146435</v>
+      </c>
+      <c r="H38" s="22">
+        <v>1871494</v>
+      </c>
+      <c r="I38" s="22">
+        <v>80678</v>
+      </c>
+      <c r="J38" s="22">
+        <v>2072</v>
+      </c>
+      <c r="K38" s="22">
+        <v>127055</v>
+      </c>
+      <c r="L38" s="22">
+        <v>5070</v>
+      </c>
+      <c r="M38" s="22">
         <f t="shared" si="11"/>
-        <v>2420237</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+        <v>2480435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B40">
-        <v>817</v>
-      </c>
-      <c r="C40">
-        <v>866</v>
-      </c>
-      <c r="D40">
-        <v>2021</v>
-      </c>
-      <c r="E40">
-        <v>2501</v>
-      </c>
-      <c r="F40">
-        <v>6315</v>
-      </c>
-      <c r="G40">
-        <v>5403</v>
-      </c>
-      <c r="H40">
-        <v>70685</v>
-      </c>
-      <c r="I40">
-        <v>567782</v>
-      </c>
-      <c r="J40">
-        <v>5390</v>
-      </c>
-      <c r="K40">
-        <v>265815</v>
-      </c>
-      <c r="L40" s="9">
+      <c r="B39" s="22">
+        <v>766</v>
+      </c>
+      <c r="C39" s="22">
+        <v>1034</v>
+      </c>
+      <c r="D39" s="22">
+        <v>2235</v>
+      </c>
+      <c r="E39" s="22">
+        <v>2997</v>
+      </c>
+      <c r="F39" s="22">
+        <v>7332</v>
+      </c>
+      <c r="G39" s="22">
+        <v>5600</v>
+      </c>
+      <c r="H39" s="22">
+        <v>80446</v>
+      </c>
+      <c r="I39" s="22">
+        <v>579051</v>
+      </c>
+      <c r="J39" s="22">
+        <v>4498</v>
+      </c>
+      <c r="K39" s="22">
+        <v>249155</v>
+      </c>
+      <c r="L39" s="22">
+        <v>18467</v>
+      </c>
+      <c r="M39" s="22">
         <f t="shared" si="11"/>
-        <v>927595</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+        <v>951581</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B41">
-        <v>218</v>
-      </c>
-      <c r="C41">
-        <v>797</v>
-      </c>
-      <c r="D41">
-        <v>706</v>
-      </c>
-      <c r="E41">
-        <v>1733</v>
-      </c>
-      <c r="F41">
-        <v>2686</v>
-      </c>
-      <c r="G41">
-        <v>1550</v>
-      </c>
-      <c r="H41">
-        <v>3143</v>
-      </c>
-      <c r="I41">
-        <v>5205</v>
-      </c>
-      <c r="J41">
-        <v>875212</v>
-      </c>
-      <c r="K41">
-        <v>25475</v>
-      </c>
-      <c r="L41" s="9">
+      <c r="B40" s="22">
+        <v>317</v>
+      </c>
+      <c r="C40" s="22">
+        <v>1108</v>
+      </c>
+      <c r="D40" s="22">
+        <v>909</v>
+      </c>
+      <c r="E40" s="22">
+        <v>2178</v>
+      </c>
+      <c r="F40" s="22">
+        <v>1694</v>
+      </c>
+      <c r="G40" s="22">
+        <v>904</v>
+      </c>
+      <c r="H40" s="22">
+        <v>1986</v>
+      </c>
+      <c r="I40" s="22">
+        <v>4453</v>
+      </c>
+      <c r="J40" s="22">
+        <v>870637</v>
+      </c>
+      <c r="K40" s="22">
+        <v>3716</v>
+      </c>
+      <c r="L40" s="22">
+        <v>25252</v>
+      </c>
+      <c r="M40" s="22">
         <f t="shared" si="11"/>
-        <v>916725</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+        <v>913154</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B42">
-        <v>1777</v>
-      </c>
-      <c r="C42">
-        <v>1693</v>
-      </c>
-      <c r="D42">
-        <v>3282</v>
-      </c>
-      <c r="E42">
-        <v>3092</v>
-      </c>
-      <c r="F42">
-        <v>9023</v>
-      </c>
-      <c r="G42">
-        <v>11534</v>
-      </c>
-      <c r="H42">
-        <v>120846</v>
-      </c>
-      <c r="I42">
-        <v>265686</v>
-      </c>
-      <c r="J42">
-        <v>25655</v>
-      </c>
-      <c r="K42">
-        <v>1588918</v>
-      </c>
-      <c r="L42" s="9">
+      <c r="B41" s="22">
+        <v>1242</v>
+      </c>
+      <c r="C41" s="22">
+        <v>1460</v>
+      </c>
+      <c r="D41" s="22">
+        <v>2878</v>
+      </c>
+      <c r="E41" s="22">
+        <v>3837</v>
+      </c>
+      <c r="F41" s="22">
+        <v>9123</v>
+      </c>
+      <c r="G41" s="22">
+        <v>9946</v>
+      </c>
+      <c r="H41" s="22">
+        <v>127067</v>
+      </c>
+      <c r="I41" s="22">
+        <v>249096</v>
+      </c>
+      <c r="J41" s="22">
+        <v>3712</v>
+      </c>
+      <c r="K41" s="22">
+        <v>1288926</v>
+      </c>
+      <c r="L41" s="22">
+        <v>13310</v>
+      </c>
+      <c r="M41" s="22">
         <f t="shared" si="11"/>
-        <v>2031506</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1710597</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B42" s="22">
+        <v>198</v>
+      </c>
+      <c r="C42" s="22">
+        <v>382</v>
+      </c>
+      <c r="D42" s="22">
+        <v>592</v>
+      </c>
+      <c r="E42" s="22">
+        <v>712</v>
+      </c>
+      <c r="F42" s="22">
+        <v>1992</v>
+      </c>
+      <c r="G42" s="22">
+        <v>1749</v>
+      </c>
+      <c r="H42" s="22">
+        <v>5049</v>
+      </c>
+      <c r="I42" s="22">
+        <v>18290</v>
+      </c>
+      <c r="J42" s="22">
+        <v>25361</v>
+      </c>
+      <c r="K42" s="22">
+        <v>13343</v>
+      </c>
+      <c r="L42" s="22">
+        <v>138204</v>
+      </c>
+      <c r="M42" s="22">
+        <f t="shared" si="11"/>
+        <v>205872</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="B43" s="11">
-        <f>SUM(B33:B42)</f>
-        <v>1591602</v>
+        <f>SUM(B32:B42)</f>
+        <v>1546882</v>
       </c>
       <c r="C43" s="11">
-        <f t="shared" ref="C43:L43" si="12">SUM(C33:C42)</f>
-        <v>1142838</v>
+        <f t="shared" ref="C43:M43" si="12">SUM(C32:C42)</f>
+        <v>1164659</v>
       </c>
       <c r="D43" s="11">
         <f t="shared" si="12"/>
-        <v>1335193</v>
+        <v>1298924</v>
       </c>
       <c r="E43" s="11">
         <f t="shared" si="12"/>
-        <v>783370</v>
+        <v>780786</v>
       </c>
       <c r="F43" s="11">
         <f t="shared" si="12"/>
-        <v>977054</v>
+        <v>984682</v>
       </c>
       <c r="G43" s="11">
         <f t="shared" si="12"/>
-        <v>2565503</v>
+        <v>2576808</v>
       </c>
       <c r="H43" s="11">
         <f t="shared" si="12"/>
-        <v>2420250</v>
+        <v>2480386</v>
       </c>
       <c r="I43" s="11">
         <f t="shared" si="12"/>
-        <v>927513</v>
+        <v>951568</v>
       </c>
       <c r="J43" s="11">
         <f t="shared" si="12"/>
-        <v>916770</v>
+        <v>913169</v>
       </c>
       <c r="K43" s="11">
         <f t="shared" si="12"/>
-        <v>2031565</v>
+        <v>1710649</v>
       </c>
       <c r="L43" s="11">
         <f t="shared" si="12"/>
-        <v>14691658</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>205857</v>
+      </c>
+      <c r="M43" s="11">
+        <f t="shared" si="12"/>
+        <v>14614370</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
+      <c r="C44" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="12"/>
@@ -4770,1231 +4861,1833 @@
       <c r="K44" s="12"/>
       <c r="L44" s="13"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+    <row r="45" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+    </row>
+    <row r="46" spans="1:13" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47" s="24">
+        <f>B32</f>
+        <v>1153569</v>
+      </c>
+      <c r="C47" s="24">
+        <f t="shared" ref="C47:K47" si="13">C32</f>
+        <v>212873</v>
+      </c>
+      <c r="D47" s="24">
+        <f t="shared" si="13"/>
+        <v>37119</v>
+      </c>
+      <c r="E47" s="24">
+        <f t="shared" si="13"/>
+        <v>9453</v>
+      </c>
+      <c r="F47" s="24">
+        <f t="shared" si="13"/>
+        <v>6572</v>
+      </c>
+      <c r="G47" s="24">
+        <f t="shared" si="13"/>
+        <v>114203</v>
+      </c>
+      <c r="H47" s="24">
+        <f t="shared" si="13"/>
+        <v>10462</v>
+      </c>
+      <c r="I47" s="24">
+        <f t="shared" si="13"/>
+        <v>785</v>
+      </c>
+      <c r="J47" s="24">
+        <f>J32+L32</f>
+        <v>498</v>
+      </c>
+      <c r="K47" s="24">
+        <f t="shared" si="13"/>
+        <v>1249</v>
+      </c>
+      <c r="L47" s="24">
+        <f>SUM(B47:K47)</f>
+        <v>1546783</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="24">
+        <f t="shared" ref="B48:K54" si="14">B33</f>
+        <v>212810</v>
+      </c>
+      <c r="C48" s="24">
+        <f t="shared" si="14"/>
+        <v>768330</v>
+      </c>
+      <c r="D48" s="24">
+        <f t="shared" si="14"/>
+        <v>93521</v>
+      </c>
+      <c r="E48" s="24">
+        <f t="shared" si="14"/>
+        <v>17006</v>
+      </c>
+      <c r="F48" s="24">
+        <f t="shared" si="14"/>
+        <v>9663</v>
+      </c>
+      <c r="G48" s="24">
+        <f t="shared" si="14"/>
+        <v>50295</v>
+      </c>
+      <c r="H48" s="24">
+        <f t="shared" si="14"/>
+        <v>9162</v>
+      </c>
+      <c r="I48" s="24">
+        <f t="shared" si="14"/>
+        <v>1042</v>
+      </c>
+      <c r="J48" s="24">
+        <f t="shared" ref="J48:J56" si="15">J33+L33</f>
+        <v>1468</v>
+      </c>
+      <c r="K48" s="24">
+        <f t="shared" si="14"/>
+        <v>1440</v>
+      </c>
+      <c r="L48" s="24">
+        <f t="shared" ref="L48:L57" si="16">SUM(B48:K48)</f>
+        <v>1164737</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="24">
+        <f t="shared" si="14"/>
+        <v>37404</v>
+      </c>
+      <c r="C49" s="24">
+        <f t="shared" si="14"/>
+        <v>93511</v>
+      </c>
+      <c r="D49" s="24">
+        <f t="shared" si="14"/>
+        <v>875899</v>
+      </c>
+      <c r="E49" s="24">
+        <f t="shared" si="14"/>
+        <v>137499</v>
+      </c>
+      <c r="F49" s="24">
+        <f t="shared" si="14"/>
+        <v>43532</v>
+      </c>
+      <c r="G49" s="24">
+        <f t="shared" si="14"/>
+        <v>78510</v>
+      </c>
+      <c r="H49" s="24">
+        <f t="shared" si="14"/>
+        <v>25960</v>
+      </c>
+      <c r="I49" s="24">
+        <f t="shared" si="14"/>
+        <v>2264</v>
+      </c>
+      <c r="J49" s="24">
+        <f t="shared" si="15"/>
+        <v>1437</v>
+      </c>
+      <c r="K49" s="24">
+        <f t="shared" si="14"/>
+        <v>2855</v>
+      </c>
+      <c r="L49" s="24">
+        <f t="shared" si="16"/>
+        <v>1298871</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="24">
+        <f t="shared" si="14"/>
+        <v>9377</v>
+      </c>
+      <c r="C50" s="24">
+        <f t="shared" si="14"/>
+        <v>16952</v>
+      </c>
+      <c r="D50" s="24">
+        <f t="shared" si="14"/>
+        <v>137988</v>
+      </c>
+      <c r="E50" s="24">
+        <f t="shared" si="14"/>
+        <v>415994</v>
+      </c>
+      <c r="F50" s="24">
+        <f t="shared" si="14"/>
+        <v>90876</v>
+      </c>
+      <c r="G50" s="24">
+        <f t="shared" si="14"/>
+        <v>63967</v>
+      </c>
+      <c r="H50" s="24">
+        <f t="shared" si="14"/>
+        <v>36004</v>
+      </c>
+      <c r="I50" s="24">
+        <f t="shared" si="14"/>
+        <v>2990</v>
+      </c>
+      <c r="J50" s="24">
+        <f t="shared" si="15"/>
+        <v>2816</v>
+      </c>
+      <c r="K50" s="24">
+        <f t="shared" si="14"/>
+        <v>3809</v>
+      </c>
+      <c r="L50" s="24">
+        <f t="shared" si="16"/>
+        <v>780773</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="24">
+        <f t="shared" si="14"/>
+        <v>6539</v>
+      </c>
+      <c r="C51" s="24">
+        <f t="shared" si="14"/>
+        <v>9562</v>
+      </c>
+      <c r="D51" s="24">
+        <f t="shared" si="14"/>
+        <v>43396</v>
+      </c>
+      <c r="E51" s="24">
+        <f t="shared" si="14"/>
+        <v>90610</v>
+      </c>
+      <c r="F51" s="24">
+        <f t="shared" si="14"/>
+        <v>583726</v>
+      </c>
+      <c r="G51" s="24">
+        <f t="shared" si="14"/>
+        <v>64524</v>
+      </c>
+      <c r="H51" s="24">
+        <f t="shared" si="14"/>
+        <v>166352</v>
+      </c>
+      <c r="I51" s="24">
+        <f t="shared" si="14"/>
+        <v>7394</v>
+      </c>
+      <c r="J51" s="24">
+        <f t="shared" si="15"/>
+        <v>3586</v>
+      </c>
+      <c r="K51" s="24">
+        <f t="shared" si="14"/>
+        <v>9047</v>
+      </c>
+      <c r="L51" s="24">
+        <f t="shared" si="16"/>
+        <v>984736</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="24">
+        <f t="shared" si="14"/>
+        <v>114301</v>
+      </c>
+      <c r="C52" s="24">
+        <f t="shared" si="14"/>
+        <v>50347</v>
+      </c>
+      <c r="D52" s="24">
+        <f t="shared" si="14"/>
+        <v>78570</v>
+      </c>
+      <c r="E52" s="24">
+        <f t="shared" si="14"/>
+        <v>64206</v>
+      </c>
+      <c r="F52" s="24">
+        <f t="shared" si="14"/>
+        <v>64111</v>
+      </c>
+      <c r="G52" s="24">
+        <f t="shared" si="14"/>
+        <v>2040675</v>
+      </c>
+      <c r="H52" s="24">
+        <f t="shared" si="14"/>
+        <v>146404</v>
+      </c>
+      <c r="I52" s="24">
+        <f t="shared" si="14"/>
+        <v>5525</v>
+      </c>
+      <c r="J52" s="24">
+        <f t="shared" si="15"/>
+        <v>2638</v>
+      </c>
+      <c r="K52" s="24">
+        <f t="shared" si="14"/>
+        <v>10054</v>
+      </c>
+      <c r="L52" s="24">
+        <f t="shared" si="16"/>
+        <v>2576831</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="24">
+        <f t="shared" si="14"/>
+        <v>10359</v>
+      </c>
+      <c r="C53" s="24">
+        <f t="shared" si="14"/>
+        <v>9100</v>
+      </c>
+      <c r="D53" s="24">
+        <f t="shared" si="14"/>
+        <v>25817</v>
+      </c>
+      <c r="E53" s="24">
+        <f t="shared" si="14"/>
+        <v>36294</v>
+      </c>
+      <c r="F53" s="24">
+        <f t="shared" si="14"/>
+        <v>166061</v>
+      </c>
+      <c r="G53" s="24">
+        <f t="shared" si="14"/>
+        <v>146435</v>
+      </c>
+      <c r="H53" s="24">
+        <f t="shared" si="14"/>
+        <v>1871494</v>
+      </c>
+      <c r="I53" s="24">
+        <f t="shared" si="14"/>
+        <v>80678</v>
+      </c>
+      <c r="J53" s="24">
+        <f t="shared" si="15"/>
+        <v>7142</v>
+      </c>
+      <c r="K53" s="24">
+        <f t="shared" si="14"/>
+        <v>127055</v>
+      </c>
+      <c r="L53" s="24">
+        <f t="shared" si="16"/>
+        <v>2480435</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="24">
+        <f t="shared" si="14"/>
+        <v>766</v>
+      </c>
+      <c r="C54" s="24">
+        <f t="shared" si="14"/>
+        <v>1034</v>
+      </c>
+      <c r="D54" s="24">
+        <f t="shared" si="14"/>
+        <v>2235</v>
+      </c>
+      <c r="E54" s="24">
+        <f t="shared" si="14"/>
+        <v>2997</v>
+      </c>
+      <c r="F54" s="24">
+        <f t="shared" si="14"/>
+        <v>7332</v>
+      </c>
+      <c r="G54" s="24">
+        <f t="shared" si="14"/>
+        <v>5600</v>
+      </c>
+      <c r="H54" s="24">
+        <f t="shared" si="14"/>
+        <v>80446</v>
+      </c>
+      <c r="I54" s="24">
+        <f t="shared" si="14"/>
+        <v>579051</v>
+      </c>
+      <c r="J54" s="24">
+        <f t="shared" si="15"/>
+        <v>22965</v>
+      </c>
+      <c r="K54" s="24">
+        <f t="shared" si="14"/>
+        <v>249155</v>
+      </c>
+      <c r="L54" s="24">
+        <f t="shared" si="16"/>
+        <v>951581</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="24">
+        <f>B40+B42</f>
+        <v>515</v>
+      </c>
+      <c r="C55" s="24">
+        <f t="shared" ref="C55:K55" si="17">C40+C42</f>
+        <v>1490</v>
+      </c>
+      <c r="D55" s="24">
+        <f t="shared" si="17"/>
+        <v>1501</v>
+      </c>
+      <c r="E55" s="24">
+        <f t="shared" si="17"/>
+        <v>2890</v>
+      </c>
+      <c r="F55" s="24">
+        <f t="shared" si="17"/>
+        <v>3686</v>
+      </c>
+      <c r="G55" s="24">
+        <f t="shared" si="17"/>
+        <v>2653</v>
+      </c>
+      <c r="H55" s="24">
+        <f t="shared" si="17"/>
+        <v>7035</v>
+      </c>
+      <c r="I55" s="24">
+        <f t="shared" si="17"/>
+        <v>22743</v>
+      </c>
+      <c r="J55" s="24">
+        <f>J40+L40+J42+L42</f>
+        <v>1059454</v>
+      </c>
+      <c r="K55" s="24">
+        <f t="shared" si="17"/>
+        <v>17059</v>
+      </c>
+      <c r="L55" s="24">
+        <f t="shared" si="16"/>
+        <v>1119026</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" s="24">
+        <f t="shared" ref="B56:K56" si="18">B41</f>
+        <v>1242</v>
+      </c>
+      <c r="C56" s="24">
+        <f t="shared" si="18"/>
+        <v>1460</v>
+      </c>
+      <c r="D56" s="24">
+        <f t="shared" si="18"/>
+        <v>2878</v>
+      </c>
+      <c r="E56" s="24">
+        <f t="shared" si="18"/>
+        <v>3837</v>
+      </c>
+      <c r="F56" s="24">
+        <f t="shared" si="18"/>
+        <v>9123</v>
+      </c>
+      <c r="G56" s="24">
+        <f t="shared" si="18"/>
+        <v>9946</v>
+      </c>
+      <c r="H56" s="24">
+        <f t="shared" si="18"/>
+        <v>127067</v>
+      </c>
+      <c r="I56" s="24">
+        <f t="shared" si="18"/>
+        <v>249096</v>
+      </c>
+      <c r="J56" s="24">
+        <f t="shared" si="15"/>
+        <v>17022</v>
+      </c>
+      <c r="K56" s="24">
+        <f t="shared" si="18"/>
+        <v>1288926</v>
+      </c>
+      <c r="L56" s="24">
+        <f t="shared" si="16"/>
+        <v>1710597</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="24">
+        <f>SUM(B47:B56)</f>
+        <v>1546882</v>
+      </c>
+      <c r="C57" s="24">
+        <f t="shared" ref="C57:K57" si="19">SUM(C47:C56)</f>
+        <v>1164659</v>
+      </c>
+      <c r="D57" s="24">
+        <f t="shared" si="19"/>
+        <v>1298924</v>
+      </c>
+      <c r="E57" s="24">
+        <f t="shared" si="19"/>
+        <v>780786</v>
+      </c>
+      <c r="F57" s="24">
+        <f t="shared" si="19"/>
+        <v>984682</v>
+      </c>
+      <c r="G57" s="24">
+        <f t="shared" si="19"/>
+        <v>2576808</v>
+      </c>
+      <c r="H57" s="24">
+        <f t="shared" si="19"/>
+        <v>2480386</v>
+      </c>
+      <c r="I57" s="24">
+        <f t="shared" si="19"/>
+        <v>951568</v>
+      </c>
+      <c r="J57" s="24">
+        <f t="shared" si="19"/>
+        <v>1119026</v>
+      </c>
+      <c r="K57" s="24">
+        <f t="shared" si="19"/>
+        <v>1710649</v>
+      </c>
+      <c r="L57" s="24">
+        <f t="shared" si="16"/>
+        <v>14614370</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="12"/>
+      <c r="L58" s="13"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="13"/>
-    </row>
-    <row r="46" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="12"/>
+      <c r="L59" s="13"/>
+    </row>
+    <row r="60" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B60" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="17"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
-      <c r="K46" s="17"/>
-      <c r="L46" s="14"/>
-    </row>
-    <row r="47" spans="1:12" ht="39" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="14"/>
+    </row>
+    <row r="61" spans="1:12" ht="39" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B61" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C47" s="10" t="s">
+      <c r="C61" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D61" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E61" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F61" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G61" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H47" s="10" t="s">
+      <c r="H61" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I47" s="10" t="s">
+      <c r="I61" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J47" s="10" t="s">
+      <c r="J61" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K47" s="10" t="s">
+      <c r="K61" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L47" s="10" t="s">
+      <c r="L61" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="11">
-        <f>B33-B18</f>
-        <v>204840.44268521119</v>
-      </c>
-      <c r="C48" s="11">
-        <f t="shared" ref="C48:L48" si="13">C33-C18</f>
-        <v>-2885.2535340450122</v>
-      </c>
-      <c r="D48" s="11">
-        <f t="shared" si="13"/>
-        <v>7565.1581695078385</v>
-      </c>
-      <c r="E48" s="11">
-        <f t="shared" si="13"/>
-        <v>-6730.1318932848226</v>
-      </c>
-      <c r="F48" s="11">
-        <f t="shared" si="13"/>
-        <v>718.08004959327991</v>
-      </c>
-      <c r="G48" s="11">
-        <f t="shared" si="13"/>
-        <v>15329.017457639056</v>
-      </c>
-      <c r="H48" s="11">
-        <f t="shared" si="13"/>
-        <v>5272.6523866288553</v>
-      </c>
-      <c r="I48" s="11">
-        <f t="shared" si="13"/>
-        <v>287.98043351999297</v>
-      </c>
-      <c r="J48" s="11">
-        <f t="shared" si="13"/>
-        <v>-1261.8241626247693</v>
-      </c>
-      <c r="K48" s="11">
-        <f t="shared" si="13"/>
-        <v>-20.178526588867953</v>
-      </c>
-      <c r="L48" s="11">
-        <f t="shared" si="13"/>
-        <v>223115.9430655567</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
+      <c r="B62" s="11">
+        <f>B47-B18</f>
+        <v>152189.23302240414</v>
+      </c>
+      <c r="C62" s="11">
+        <f>C47-C18</f>
+        <v>7943.5147063495824</v>
+      </c>
+      <c r="D62" s="11">
+        <f>D47-D18</f>
+        <v>8176.2218620737185</v>
+      </c>
+      <c r="E62" s="11">
+        <f>E47-E18</f>
+        <v>-4447.6185630828677</v>
+      </c>
+      <c r="F62" s="11">
+        <f>F47-F18</f>
+        <v>1517.8091050291632</v>
+      </c>
+      <c r="G62" s="11">
+        <f>G47-G18</f>
+        <v>13906.435183584894</v>
+      </c>
+      <c r="H62" s="11">
+        <f>H47-H18</f>
+        <v>7503.2994550769654</v>
+      </c>
+      <c r="I62" s="11">
+        <f>I47-I18</f>
+        <v>249.81077821315876</v>
+      </c>
+      <c r="J62" s="11">
+        <f>J47-J18</f>
+        <v>-934.24971936717748</v>
+      </c>
+      <c r="K62" s="11">
+        <f>K47-K18</f>
+        <v>-542.7031163960221</v>
+      </c>
+      <c r="L62" s="11">
+        <f t="shared" ref="L62" si="20">L47-L18</f>
+        <v>185561.75271388562</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="11">
-        <f t="shared" ref="B49:L49" si="14">B34-B19</f>
-        <v>-2106.3406709801056</v>
-      </c>
-      <c r="C49" s="11">
-        <f t="shared" si="14"/>
-        <v>-125756.18961327744</v>
-      </c>
-      <c r="D49" s="11">
-        <f t="shared" si="14"/>
-        <v>9657.5733846295479</v>
-      </c>
-      <c r="E49" s="11">
-        <f t="shared" si="14"/>
-        <v>-8088.4511454875792</v>
-      </c>
-      <c r="F49" s="11">
-        <f t="shared" si="14"/>
-        <v>587.11809448538588</v>
-      </c>
-      <c r="G49" s="11">
-        <f t="shared" si="14"/>
-        <v>5531.21951066365</v>
-      </c>
-      <c r="H49" s="11">
-        <f t="shared" si="14"/>
-        <v>1176.6967334883166</v>
-      </c>
-      <c r="I49" s="11">
-        <f t="shared" si="14"/>
-        <v>-2098.6914773175968</v>
-      </c>
-      <c r="J49" s="11">
-        <f t="shared" si="14"/>
-        <v>-4257.9094828765137</v>
-      </c>
-      <c r="K49" s="11">
-        <f t="shared" si="14"/>
-        <v>1362.9537049394603</v>
-      </c>
-      <c r="L49" s="11">
-        <f t="shared" si="14"/>
-        <v>-123992.0209617326</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+      <c r="B63" s="11">
+        <f>B48-B19</f>
+        <v>8943.8043689996412</v>
+      </c>
+      <c r="C63" s="11">
+        <f>C48-C19</f>
+        <v>-113033.10659822018</v>
+      </c>
+      <c r="D63" s="11">
+        <f>D48-D19</f>
+        <v>7723.313885548414</v>
+      </c>
+      <c r="E63" s="11">
+        <f>E48-E19</f>
+        <v>-5402.9416046221122</v>
+      </c>
+      <c r="F63" s="11">
+        <f>F48-F19</f>
+        <v>2050.3773992359738</v>
+      </c>
+      <c r="G63" s="11">
+        <f>G48-G19</f>
+        <v>5670.2173811871689</v>
+      </c>
+      <c r="H63" s="11">
+        <f>H48-H19</f>
+        <v>2832.1719874632017</v>
+      </c>
+      <c r="I63" s="11">
+        <f>I48-I19</f>
+        <v>-1953.8479550344805</v>
+      </c>
+      <c r="J63" s="11">
+        <f>J48-J19</f>
+        <v>-3410.1116215246793</v>
+      </c>
+      <c r="K63" s="11">
+        <f>K48-K19</f>
+        <v>1116.6636670181201</v>
+      </c>
+      <c r="L63" s="11">
+        <f t="shared" ref="L63" si="21">L48-L19</f>
+        <v>-95463.459089948796</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="11">
-        <f t="shared" ref="B50:L50" si="15">B35-B20</f>
-        <v>4232.3946962727787</v>
-      </c>
-      <c r="C50" s="11">
-        <f t="shared" si="15"/>
-        <v>7534.8480599474715</v>
-      </c>
-      <c r="D50" s="11">
-        <f t="shared" si="15"/>
-        <v>-399393.32948769652</v>
-      </c>
-      <c r="E50" s="11">
-        <f t="shared" si="15"/>
-        <v>-57059.972243686469</v>
-      </c>
-      <c r="F50" s="11">
-        <f t="shared" si="15"/>
-        <v>-14455.416346276841</v>
-      </c>
-      <c r="G50" s="11">
-        <f t="shared" si="15"/>
-        <v>9828.2299141909607</v>
-      </c>
-      <c r="H50" s="11">
-        <f t="shared" si="15"/>
-        <v>-8509.2261959790376</v>
-      </c>
-      <c r="I50" s="11">
-        <f t="shared" si="15"/>
-        <v>-151.83447339367785</v>
-      </c>
-      <c r="J50" s="11">
-        <f t="shared" si="15"/>
-        <v>-3159.0876572567872</v>
-      </c>
-      <c r="K50" s="11">
-        <f t="shared" si="15"/>
-        <v>1581.0232932010924</v>
-      </c>
-      <c r="L50" s="11">
-        <f t="shared" si="15"/>
-        <v>-459552.37044067681</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
+      <c r="B64" s="11">
+        <f>B49-B20</f>
+        <v>4905.2640484394651</v>
+      </c>
+      <c r="C64" s="11">
+        <f>C49-C20</f>
+        <v>5871.3298812056892</v>
+      </c>
+      <c r="D64" s="11">
+        <f>D49-D20</f>
+        <v>-449825.2455007534</v>
+      </c>
+      <c r="E64" s="11">
+        <f>E49-E20</f>
+        <v>-47109.670499201951</v>
+      </c>
+      <c r="F64" s="11">
+        <f>F49-F20</f>
+        <v>-7461.7363059048803</v>
+      </c>
+      <c r="G64" s="11">
+        <f>G49-G20</f>
+        <v>12206.873563967718</v>
+      </c>
+      <c r="H64" s="11">
+        <f>H49-H20</f>
+        <v>-3907.2733167168881</v>
+      </c>
+      <c r="I64" s="11">
+        <f>I49-I20</f>
+        <v>92.648703711292001</v>
+      </c>
+      <c r="J64" s="11">
+        <f>J49-J20</f>
+        <v>-2378.9072567292183</v>
+      </c>
+      <c r="K64" s="11">
+        <f>K49-K20</f>
+        <v>1135.1188732721146</v>
+      </c>
+      <c r="L64" s="11">
+        <f t="shared" ref="L64" si="22">L49-L20</f>
+        <v>-486471.59780870983</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="11">
-        <f t="shared" ref="B51:L51" si="16">B36-B21</f>
-        <v>-7927.4379608868803</v>
-      </c>
-      <c r="C51" s="11">
-        <f t="shared" si="16"/>
-        <v>-6640.3840071530431</v>
-      </c>
-      <c r="D51" s="11">
-        <f t="shared" si="16"/>
-        <v>-59934.916623309342</v>
-      </c>
-      <c r="E51" s="11">
-        <f t="shared" si="16"/>
-        <v>-146448.93115436402</v>
-      </c>
-      <c r="F51" s="11">
-        <f t="shared" si="16"/>
-        <v>-12351.155550266281</v>
-      </c>
-      <c r="G51" s="11">
-        <f t="shared" si="16"/>
-        <v>-26666.949883066642</v>
-      </c>
-      <c r="H51" s="11">
-        <f t="shared" si="16"/>
-        <v>-6824.6624675190469</v>
-      </c>
-      <c r="I51" s="11">
-        <f t="shared" si="16"/>
-        <v>-2899.1178753624936</v>
-      </c>
-      <c r="J51" s="11">
-        <f t="shared" si="16"/>
-        <v>-7384.9092673388968</v>
-      </c>
-      <c r="K51" s="11">
-        <f t="shared" si="16"/>
-        <v>-1793.4348482912137</v>
-      </c>
-      <c r="L51" s="11">
-        <f t="shared" si="16"/>
-        <v>-278871.8996375578</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="B65" s="11">
+        <f>B50-B21</f>
+        <v>-5700.6996450942715</v>
+      </c>
+      <c r="C65" s="11">
+        <f>C50-C21</f>
+        <v>-3925.9709943300622</v>
+      </c>
+      <c r="D65" s="11">
+        <f>D50-D21</f>
+        <v>-49993.776231259486</v>
+      </c>
+      <c r="E65" s="11">
+        <f>E50-E21</f>
+        <v>-171036.42459975614</v>
+      </c>
+      <c r="F65" s="11">
+        <f>F50-F21</f>
+        <v>-6670.2826734154223</v>
+      </c>
+      <c r="G65" s="11">
+        <f>G50-G21</f>
+        <v>-27607.65790468255</v>
+      </c>
+      <c r="H65" s="11">
+        <f>H50-H21</f>
+        <v>-1337.1838613066211</v>
+      </c>
+      <c r="I65" s="11">
+        <f>I50-I21</f>
+        <v>-2365.7937949659172</v>
+      </c>
+      <c r="J65" s="11">
+        <f>J50-J21</f>
+        <v>-6166.4058727285592</v>
+      </c>
+      <c r="K65" s="11">
+        <f>K50-K21</f>
+        <v>-1064.6605265261196</v>
+      </c>
+      <c r="L65" s="11">
+        <f t="shared" ref="L65" si="23">L50-L21</f>
+        <v>-275868.8561040652</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B52" s="11">
-        <f t="shared" ref="B52:L52" si="17">B37-B22</f>
-        <v>-894.1294196088038</v>
-      </c>
-      <c r="C52" s="11">
-        <f t="shared" si="17"/>
-        <v>1164.4319517558206</v>
-      </c>
-      <c r="D52" s="11">
-        <f t="shared" si="17"/>
-        <v>-18069.135233888555</v>
-      </c>
-      <c r="E52" s="11">
-        <f t="shared" si="17"/>
-        <v>-9001.6440433993266</v>
-      </c>
-      <c r="F52" s="11">
-        <f t="shared" si="17"/>
-        <v>35844.940627612988</v>
-      </c>
-      <c r="G52" s="11">
-        <f t="shared" si="17"/>
-        <v>29448.691080151126</v>
-      </c>
-      <c r="H52" s="11">
-        <f t="shared" si="17"/>
-        <v>53572.376332653395</v>
-      </c>
-      <c r="I52" s="11">
-        <f t="shared" si="17"/>
-        <v>-529.53562875909211</v>
-      </c>
-      <c r="J52" s="11">
-        <f t="shared" si="17"/>
-        <v>9.2900329184994916</v>
-      </c>
-      <c r="K52" s="11">
-        <f t="shared" si="17"/>
-        <v>70.277627493704131</v>
-      </c>
-      <c r="L52" s="11">
-        <f t="shared" si="17"/>
-        <v>91615.563326929696</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="B66" s="11">
+        <f>B51-B22</f>
+        <v>-33.371476115787118</v>
+      </c>
+      <c r="C66" s="11">
+        <f>C51-C22</f>
+        <v>2666.8966605934947</v>
+      </c>
+      <c r="D66" s="11">
+        <f>D51-D22</f>
+        <v>-10912.922851191055</v>
+      </c>
+      <c r="E66" s="11">
+        <f>E51-E22</f>
+        <v>-3350.7333208092459</v>
+      </c>
+      <c r="F66" s="11">
+        <f>F51-F22</f>
+        <v>19635.131490126485</v>
+      </c>
+      <c r="G66" s="11">
+        <f>G51-G22</f>
+        <v>30211.15433962785</v>
+      </c>
+      <c r="H66" s="11">
+        <f>H51-H22</f>
+        <v>63884.276218561572</v>
+      </c>
+      <c r="I66" s="11">
+        <f>I51-I22</f>
+        <v>529.76582868536661</v>
+      </c>
+      <c r="J66" s="11">
+        <f>J51-J22</f>
+        <v>1095.4612308823916</v>
+      </c>
+      <c r="K66" s="11">
+        <f>K51-K22</f>
+        <v>195.09089082492756</v>
+      </c>
+      <c r="L66" s="11">
+        <f t="shared" ref="L66" si="24">L51-L22</f>
+        <v>103920.74901118595</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="11">
-        <f t="shared" ref="B53:L53" si="18">B38-B23</f>
-        <v>18468.482582812299</v>
-      </c>
-      <c r="C53" s="11">
-        <f t="shared" si="18"/>
-        <v>7040.3337067295797</v>
-      </c>
-      <c r="D53" s="11">
-        <f t="shared" si="18"/>
-        <v>6168.4909841394547</v>
-      </c>
-      <c r="E53" s="11">
-        <f t="shared" si="18"/>
-        <v>-31688.325637437985</v>
-      </c>
-      <c r="F53" s="11">
-        <f t="shared" si="18"/>
-        <v>27122.203381131054</v>
-      </c>
-      <c r="G53" s="11">
-        <f t="shared" si="18"/>
-        <v>-195362.04605364427</v>
-      </c>
-      <c r="H53" s="11">
-        <f t="shared" si="18"/>
-        <v>40371.319224575273</v>
-      </c>
-      <c r="I53" s="11">
-        <f t="shared" si="18"/>
-        <v>370.35738679065344</v>
-      </c>
-      <c r="J53" s="11">
-        <f t="shared" si="18"/>
-        <v>-957.27591499389155</v>
-      </c>
-      <c r="K53" s="11">
-        <f t="shared" si="18"/>
-        <v>5086.0856481887613</v>
-      </c>
-      <c r="L53" s="11">
-        <f t="shared" si="18"/>
-        <v>-123380.37469170894</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
+      <c r="B67" s="11">
+        <f>B52-B23</f>
+        <v>16876.710300619205</v>
+      </c>
+      <c r="C67" s="11">
+        <f>C52-C23</f>
+        <v>7203.4978352761536</v>
+      </c>
+      <c r="D67" s="11">
+        <f>D52-D23</f>
+        <v>8811.4088364892668</v>
+      </c>
+      <c r="E67" s="11">
+        <f>E52-E23</f>
+        <v>-32667.013341040511</v>
+      </c>
+      <c r="F67" s="11">
+        <f>F52-F23</f>
+        <v>28077.764908841484</v>
+      </c>
+      <c r="G67" s="11">
+        <f>G52-G23</f>
+        <v>-177357.99310091464</v>
+      </c>
+      <c r="H67" s="11">
+        <f>H52-H23</f>
+        <v>46956.248009452451</v>
+      </c>
+      <c r="I67" s="11">
+        <f>I52-I23</f>
+        <v>461.13758997056084</v>
+      </c>
+      <c r="J67" s="11">
+        <f>J52-J23</f>
+        <v>168.78252544339966</v>
+      </c>
+      <c r="K67" s="11">
+        <f>K52-K23</f>
+        <v>3558.4373885044424</v>
+      </c>
+      <c r="L67" s="11">
+        <f t="shared" ref="L67" si="25">L52-L23</f>
+        <v>-97911.019047358539</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="11">
-        <f t="shared" ref="B54:L54" si="19">B39-B24</f>
-        <v>4469.0200362412434</v>
-      </c>
-      <c r="C54" s="11">
-        <f t="shared" si="19"/>
-        <v>1789.9871619319965</v>
-      </c>
-      <c r="D54" s="11">
-        <f t="shared" si="19"/>
-        <v>-3310.102418804956</v>
-      </c>
-      <c r="E54" s="11">
-        <f t="shared" si="19"/>
-        <v>-7832.2907121654425</v>
-      </c>
-      <c r="F54" s="11">
-        <f t="shared" si="19"/>
-        <v>52694.421881025482</v>
-      </c>
-      <c r="G54" s="11">
-        <f t="shared" si="19"/>
-        <v>35626.814814833939</v>
-      </c>
-      <c r="H54" s="11">
-        <f t="shared" si="19"/>
-        <v>396556.18799074227</v>
-      </c>
-      <c r="I54" s="11">
-        <f t="shared" si="19"/>
-        <v>10042.166120494774</v>
-      </c>
-      <c r="J54" s="11">
-        <f t="shared" si="19"/>
-        <v>20.601579995428438</v>
-      </c>
-      <c r="K54" s="11">
-        <f t="shared" si="19"/>
-        <v>21816.491070176649</v>
-      </c>
-      <c r="L54" s="11">
-        <f t="shared" si="19"/>
-        <v>511873.29752447107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="B68" s="11">
+        <f>B53-B24</f>
+        <v>6665.5528075213115</v>
+      </c>
+      <c r="C68" s="11">
+        <f>C53-C24</f>
+        <v>3328.5096508320648</v>
+      </c>
+      <c r="D68" s="11">
+        <f>D53-D24</f>
+        <v>1228.9314207892276</v>
+      </c>
+      <c r="E68" s="11">
+        <f>E53-E24</f>
+        <v>-2331.0225335458599</v>
+      </c>
+      <c r="F68" s="11">
+        <f>F53-F24</f>
+        <v>63092.967645544311</v>
+      </c>
+      <c r="G68" s="11">
+        <f>G53-G24</f>
+        <v>42362.203119311976</v>
+      </c>
+      <c r="H68" s="11">
+        <f>H53-H24</f>
+        <v>415120.21123131667</v>
+      </c>
+      <c r="I68" s="11">
+        <f>I53-I24</f>
+        <v>20286.54592969529</v>
+      </c>
+      <c r="J68" s="11">
+        <f>J53-J24</f>
+        <v>3851.0059803078584</v>
+      </c>
+      <c r="K68" s="11">
+        <f>K53-K24</f>
+        <v>28505.668563837899</v>
+      </c>
+      <c r="L68" s="11">
+        <f t="shared" ref="L68" si="26">L53-L24</f>
+        <v>582110.57381561026</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="11">
-        <f t="shared" ref="B55:L55" si="20">B40-B25</f>
-        <v>-397.07608567628267</v>
-      </c>
-      <c r="C55" s="11">
-        <f t="shared" si="20"/>
-        <v>-1296.9472085701236</v>
-      </c>
-      <c r="D55" s="11">
-        <f t="shared" si="20"/>
-        <v>-1178.1565694807409</v>
-      </c>
-      <c r="E55" s="11">
-        <f t="shared" si="20"/>
-        <v>-2603.5913197869786</v>
-      </c>
-      <c r="F55" s="11">
-        <f t="shared" si="20"/>
-        <v>131.4140787306178</v>
-      </c>
-      <c r="G55" s="11">
-        <f t="shared" si="20"/>
-        <v>1730.706065526098</v>
-      </c>
-      <c r="H55" s="11">
-        <f t="shared" si="20"/>
-        <v>11710.628172803656</v>
-      </c>
-      <c r="I55" s="11">
-        <f t="shared" si="20"/>
-        <v>-124003.09454381384</v>
-      </c>
-      <c r="J55" s="11">
-        <f t="shared" si="20"/>
-        <v>-3444.4478374446117</v>
-      </c>
-      <c r="K55" s="11">
-        <f t="shared" si="20"/>
-        <v>59389.941978101706</v>
-      </c>
-      <c r="L55" s="11">
-        <f t="shared" si="20"/>
-        <v>-59960.623269610456</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="B69" s="11">
+        <f>B54-B25</f>
+        <v>-441.6892291002755</v>
+      </c>
+      <c r="C69" s="11">
+        <f>C54-C25</f>
+        <v>-1117.5686518506595</v>
+      </c>
+      <c r="D69" s="11">
+        <f>D54-D25</f>
+        <v>-947.32685475813923</v>
+      </c>
+      <c r="E69" s="11">
+        <f>E54-E25</f>
+        <v>-2080.7377370311251</v>
+      </c>
+      <c r="F69" s="11">
+        <f>F54-F25</f>
+        <v>1180.9438986245377</v>
+      </c>
+      <c r="G69" s="11">
+        <f>G54-G25</f>
+        <v>1947.0248009341517</v>
+      </c>
+      <c r="H69" s="11">
+        <f>H54-H25</f>
+        <v>21781.873023982487</v>
+      </c>
+      <c r="I69" s="11">
+        <f>I54-I25</f>
+        <v>-109094.83977848361</v>
+      </c>
+      <c r="J69" s="11">
+        <f>J54-J25</f>
+        <v>14177.027298612898</v>
+      </c>
+      <c r="K69" s="11">
+        <f>K54-K25</f>
+        <v>43815.876587006729</v>
+      </c>
+      <c r="L69" s="11">
+        <f t="shared" ref="L69" si="27">L54-L25</f>
+        <v>-30779.416642062948</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="11">
-        <f t="shared" ref="B56:L56" si="21">B41-B26</f>
-        <v>-1298.8596926148989</v>
-      </c>
-      <c r="C56" s="11">
-        <f t="shared" si="21"/>
-        <v>-3763.4122254518988</v>
-      </c>
-      <c r="D56" s="11">
-        <f t="shared" si="21"/>
-        <v>-2665.3885692130657</v>
-      </c>
-      <c r="E56" s="11">
-        <f t="shared" si="21"/>
-        <v>-6889.6898988754729</v>
-      </c>
-      <c r="F56" s="11">
-        <f t="shared" si="21"/>
-        <v>721.26253083796882</v>
-      </c>
-      <c r="G56" s="11">
-        <f t="shared" si="21"/>
-        <v>-640.02979629164429</v>
-      </c>
-      <c r="H56" s="11">
-        <f t="shared" si="21"/>
-        <v>-228.7062130262193</v>
-      </c>
-      <c r="I56" s="11">
-        <f t="shared" si="21"/>
-        <v>-2963.459246065263</v>
-      </c>
-      <c r="J56" s="11">
-        <f t="shared" si="21"/>
-        <v>-1473.8343927654205</v>
-      </c>
-      <c r="K56" s="11">
-        <f t="shared" si="21"/>
-        <v>1293.6741936235776</v>
-      </c>
-      <c r="L56" s="11">
-        <f t="shared" si="21"/>
-        <v>-17908.443309842376</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="B70" s="11">
+        <f>B55-B26</f>
+        <v>-993.87999066956218</v>
+      </c>
+      <c r="C70" s="11">
+        <f>C55-C26</f>
+        <v>-3046.4213906474997</v>
+      </c>
+      <c r="D70" s="11">
+        <f>D55-D26</f>
+        <v>-1852.6527983601541</v>
+      </c>
+      <c r="E70" s="11">
+        <f>E55-E26</f>
+        <v>-5687.3287519644655</v>
+      </c>
+      <c r="F70" s="11">
+        <f>F55-F26</f>
+        <v>1731.5983710485559</v>
+      </c>
+      <c r="G70" s="11">
+        <f>G55-G26</f>
+        <v>474.49123305002604</v>
+      </c>
+      <c r="H70" s="11">
+        <f>H55-H26</f>
+        <v>3681.031228846738</v>
+      </c>
+      <c r="I70" s="11">
+        <f>I55-I26</f>
+        <v>14617.512342179569</v>
+      </c>
+      <c r="J70" s="11">
+        <f>J55-J26</f>
+        <v>187380.12259456352</v>
+      </c>
+      <c r="K70" s="11">
+        <f>K55-K26</f>
+        <v>-6995.1157727013124</v>
+      </c>
+      <c r="L70" s="11">
+        <f t="shared" ref="L70" si="28">L55-L26</f>
+        <v>189309.35706534551</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="11">
-        <f t="shared" ref="B57:L57" si="22">B42-B27</f>
-        <v>211.37507676567702</v>
-      </c>
-      <c r="C57" s="11">
-        <f t="shared" si="22"/>
-        <v>1435.8742385521275</v>
-      </c>
-      <c r="D57" s="11">
-        <f t="shared" si="22"/>
-        <v>1190.4812175878092</v>
-      </c>
-      <c r="E57" s="11">
-        <f t="shared" si="22"/>
-        <v>-2074.7804541623018</v>
-      </c>
-      <c r="F57" s="11">
-        <f t="shared" si="22"/>
-        <v>2487.3404383508441</v>
-      </c>
-      <c r="G57" s="11">
-        <f t="shared" si="22"/>
-        <v>4516.3090465893711</v>
-      </c>
-      <c r="H57" s="11">
-        <f t="shared" si="22"/>
-        <v>16862.397537919809</v>
-      </c>
-      <c r="I57" s="11">
-        <f t="shared" si="22"/>
-        <v>64362.895473179437</v>
-      </c>
-      <c r="J57" s="11">
-        <f t="shared" si="22"/>
-        <v>1031.9835661326615</v>
-      </c>
-      <c r="K57" s="11">
-        <f t="shared" si="22"/>
-        <v>147037.05225325702</v>
-      </c>
-      <c r="L57" s="11">
-        <f t="shared" si="22"/>
-        <v>237060.92839417257</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="B71" s="11">
+        <f>B56-B27</f>
+        <v>-315.38868338536008</v>
+      </c>
+      <c r="C71" s="11">
+        <f>C56-C27</f>
+        <v>1204.226892953066</v>
+      </c>
+      <c r="D71" s="11">
+        <f>D56-D27</f>
+        <v>797.48401275599736</v>
+      </c>
+      <c r="E71" s="11">
+        <f>E56-E27</f>
+        <v>-1302.599714742606</v>
+      </c>
+      <c r="F71" s="11">
+        <f>F56-F27</f>
+        <v>2621.7224023334493</v>
+      </c>
+      <c r="G71" s="11">
+        <f>G56-G27</f>
+        <v>2965.2268198187239</v>
+      </c>
+      <c r="H71" s="11">
+        <f>H56-H27</f>
+        <v>23630.421207208143</v>
+      </c>
+      <c r="I71" s="11">
+        <f>I56-I27</f>
+        <v>48831.990376060305</v>
+      </c>
+      <c r="J71" s="11">
+        <f>J56-J27</f>
+        <v>-7471.4828104913577</v>
+      </c>
+      <c r="K71" s="11">
+        <f>K56-K27</f>
+        <v>-145369.68441639259</v>
+      </c>
+      <c r="L71" s="11">
+        <f t="shared" ref="L71" si="29">L56-L27</f>
+        <v>-74408.08391388203</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B58" s="11">
-        <f t="shared" ref="B58:L58" si="23">B43-B28</f>
-        <v>219597.87124753627</v>
-      </c>
-      <c r="C58" s="11">
-        <f t="shared" si="23"/>
-        <v>-121376.71146958065</v>
-      </c>
-      <c r="D58" s="11">
-        <f t="shared" si="23"/>
-        <v>-459969.32514652819</v>
-      </c>
-      <c r="E58" s="11">
-        <f t="shared" si="23"/>
-        <v>-278417.80850265059</v>
-      </c>
-      <c r="F58" s="11">
-        <f t="shared" si="23"/>
-        <v>93500.209185224492</v>
-      </c>
-      <c r="G58" s="11">
-        <f t="shared" si="23"/>
-        <v>-120658.03784340806</v>
-      </c>
-      <c r="H58" s="11">
-        <f t="shared" si="23"/>
-        <v>509959.66350228735</v>
-      </c>
-      <c r="I58" s="11">
-        <f t="shared" si="23"/>
-        <v>-57582.333830727148</v>
-      </c>
-      <c r="J58" s="11">
-        <f t="shared" si="23"/>
-        <v>-20877.4135362542</v>
-      </c>
-      <c r="K58" s="11">
-        <f t="shared" si="23"/>
-        <v>235823.88639410166</v>
-      </c>
-      <c r="L58" s="11">
-        <f t="shared" si="23"/>
+      <c r="B72" s="11">
+        <f>B57-B28</f>
+        <v>182095.53552361857</v>
+      </c>
+      <c r="C72" s="11">
+        <f>C57-C28</f>
+        <v>-92905.092007838422</v>
+      </c>
+      <c r="D72" s="11">
+        <f>D57-D28</f>
+        <v>-486794.56421866524</v>
+      </c>
+      <c r="E72" s="11">
+        <f>E57-E28</f>
+        <v>-275416.090665797</v>
+      </c>
+      <c r="F72" s="11">
+        <f>F57-F28</f>
+        <v>105776.29624146363</v>
+      </c>
+      <c r="G72" s="11">
+        <f>G57-G28</f>
+        <v>-95222.024564114399</v>
+      </c>
+      <c r="H72" s="11">
+        <f>H57-H28</f>
+        <v>580145.07518388494</v>
+      </c>
+      <c r="I72" s="11">
+        <f>I57-I28</f>
+        <v>-28345.069979968481</v>
+      </c>
+      <c r="J72" s="11">
+        <f>J57-J28</f>
+        <v>186311.24234896922</v>
+      </c>
+      <c r="K72" s="11">
+        <f>K57-K28</f>
+        <v>-75645.307861552108</v>
+      </c>
+      <c r="L72" s="11">
+        <f t="shared" ref="L72" si="30">L57-L28</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="12"/>
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
-      <c r="H60" s="12"/>
-      <c r="I60" s="12"/>
-      <c r="J60" s="12"/>
-      <c r="K60" s="12"/>
-      <c r="L60" s="13"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="13"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B75" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
-      <c r="J61" s="17"/>
-      <c r="K61" s="17"/>
-      <c r="L61" s="14"/>
-    </row>
-    <row r="62" spans="1:14" ht="39" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+      <c r="F75" s="17"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="14"/>
+    </row>
+    <row r="76" spans="1:14" ht="39" x14ac:dyDescent="0.25">
+      <c r="A76" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C62" s="10" t="s">
+      <c r="C76" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D76" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E76" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="F62" s="10" t="s">
+      <c r="F76" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G62" s="10" t="s">
+      <c r="G76" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H62" s="10" t="s">
+      <c r="H76" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="I62" s="10" t="s">
+      <c r="I76" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J62" s="10" t="s">
+      <c r="J76" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K62" s="10" t="s">
+      <c r="K76" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L62" s="10" t="s">
+      <c r="L76" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="20">
-        <f>B48/B5</f>
-        <v>0.28102098181913304</v>
-      </c>
-      <c r="C63" s="20">
-        <f t="shared" ref="C63:L63" si="24">C48/C5</f>
-        <v>-1.9342000295534623E-2</v>
-      </c>
-      <c r="D63" s="20">
-        <f t="shared" si="24"/>
-        <v>0.35908697315271482</v>
-      </c>
-      <c r="E63" s="20">
-        <f t="shared" si="24"/>
-        <v>-0.66513729857604331</v>
-      </c>
-      <c r="F63" s="20">
-        <f t="shared" si="24"/>
-        <v>0.19518348725014403</v>
-      </c>
-      <c r="G63" s="20">
-        <f t="shared" si="24"/>
-        <v>0.20996655054948957</v>
-      </c>
-      <c r="H63" s="20">
-        <f t="shared" si="24"/>
-        <v>2.4482174087157529</v>
-      </c>
-      <c r="I63" s="20">
-        <f t="shared" si="24"/>
-        <v>0.73922641250607846</v>
-      </c>
-      <c r="J63" s="20">
-        <f t="shared" si="24"/>
-        <v>-1.2103248406549032</v>
-      </c>
-      <c r="K63" s="20">
-        <f t="shared" si="24"/>
-        <v>-1.5471957206615513E-2</v>
-      </c>
-      <c r="L63" s="20">
-        <f t="shared" si="24"/>
-        <v>0.22517684941033134</v>
-      </c>
-      <c r="N63" s="21"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="9" t="s">
+      <c r="B77" s="20">
+        <f>B62/B5</f>
+        <v>0.20878868999507672</v>
+      </c>
+      <c r="C77" s="20">
+        <f>C62/C5</f>
+        <v>5.3251286926731582E-2</v>
+      </c>
+      <c r="D77" s="20">
+        <f>D62/D5</f>
+        <v>0.38809165578465482</v>
+      </c>
+      <c r="E77" s="20">
+        <f>E62/E5</f>
+        <v>-0.4395570611472423</v>
+      </c>
+      <c r="F77" s="20">
+        <f>F62/F5</f>
+        <v>0.41256023512616558</v>
+      </c>
+      <c r="G77" s="20">
+        <f>G62/G5</f>
+        <v>0.19048097727113505</v>
+      </c>
+      <c r="H77" s="20">
+        <f>H62/H5</f>
+        <v>3.4839596851314107</v>
+      </c>
+      <c r="I77" s="20">
+        <f>I62/I5</f>
+        <v>0.64124747340185018</v>
+      </c>
+      <c r="J77" s="20">
+        <f>J62/J5</f>
+        <v>-0.89611982098429577</v>
+      </c>
+      <c r="K77" s="20">
+        <f>K62/K5</f>
+        <v>-0.41611954945255486</v>
+      </c>
+      <c r="L77" s="20">
+        <f t="shared" ref="L77" si="31">L62/L5</f>
+        <v>0.1872757736317148</v>
+      </c>
+      <c r="N77" s="21"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="20">
-        <f t="shared" ref="B64:L64" si="25">B49/B6</f>
-        <v>-1.4194014618818959E-2</v>
-      </c>
-      <c r="C64" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.19601818150729619</v>
-      </c>
-      <c r="D64" s="20">
-        <f t="shared" si="25"/>
-        <v>0.15463731296159947</v>
-      </c>
-      <c r="E64" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.49586776282116218</v>
-      </c>
-      <c r="F64" s="20">
-        <f t="shared" si="25"/>
-        <v>0.10595294154006649</v>
-      </c>
-      <c r="G64" s="20">
-        <f t="shared" si="25"/>
-        <v>0.17028117322993264</v>
-      </c>
-      <c r="H64" s="20">
-        <f t="shared" si="25"/>
-        <v>0.25538447406719766</v>
-      </c>
-      <c r="I64" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.96238907388767725</v>
-      </c>
-      <c r="J64" s="20">
-        <f t="shared" si="25"/>
-        <v>-1.1991307617871072</v>
-      </c>
-      <c r="K64" s="20">
-        <f t="shared" si="25"/>
-        <v>5.7909317850928801</v>
-      </c>
-      <c r="L64" s="20">
-        <f t="shared" si="25"/>
-        <v>-0.13516864443117763</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="9" t="s">
+      <c r="B78" s="20">
+        <f>B63/B6</f>
+        <v>6.0269685578623479E-2</v>
+      </c>
+      <c r="C78" s="20">
+        <f>C63/C6</f>
+        <v>-0.17618650878051237</v>
+      </c>
+      <c r="D78" s="20">
+        <f>D63/D6</f>
+        <v>0.12366590020646569</v>
+      </c>
+      <c r="E78" s="20">
+        <f>E63/E6</f>
+        <v>-0.33123085222960147</v>
+      </c>
+      <c r="F78" s="20">
+        <f>F63/F6</f>
+        <v>0.37001672875835745</v>
+      </c>
+      <c r="G78" s="20">
+        <f>G63/G6</f>
+        <v>0.17456028752354838</v>
+      </c>
+      <c r="H78" s="20">
+        <f>H63/H6</f>
+        <v>0.61468068441214996</v>
+      </c>
+      <c r="I78" s="20">
+        <f>I63/I6</f>
+        <v>-0.89596872350495038</v>
+      </c>
+      <c r="J78" s="20">
+        <f>J63/J6</f>
+        <v>-0.96037028568663652</v>
+      </c>
+      <c r="K78" s="20">
+        <f>K63/K6</f>
+        <v>4.7444921270314415</v>
+      </c>
+      <c r="L78" s="20">
+        <f t="shared" ref="L78" si="32">L63/L6</f>
+        <v>-0.10406852197273236</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="20">
-        <f t="shared" ref="B65:L65" si="26">B50/B7</f>
-        <v>0.17891285474970087</v>
-      </c>
-      <c r="C65" s="20">
-        <f t="shared" si="26"/>
-        <v>0.11811243370361146</v>
-      </c>
-      <c r="D65" s="20">
-        <f t="shared" si="26"/>
-        <v>-0.41387525509369044</v>
-      </c>
-      <c r="E65" s="20">
-        <f t="shared" si="26"/>
-        <v>-0.42462084929335842</v>
-      </c>
-      <c r="F65" s="20">
-        <f t="shared" si="26"/>
-        <v>-0.38943557704114645</v>
-      </c>
-      <c r="G65" s="20">
-        <f t="shared" si="26"/>
-        <v>0.20364003041249526</v>
-      </c>
-      <c r="H65" s="20">
-        <f t="shared" si="26"/>
-        <v>-0.3913959661841328</v>
-      </c>
-      <c r="I65" s="20">
-        <f t="shared" si="26"/>
-        <v>-9.6064327856554901E-2</v>
-      </c>
-      <c r="J65" s="20">
-        <f t="shared" si="26"/>
-        <v>-1.1373279680796602</v>
-      </c>
-      <c r="K65" s="20">
-        <f t="shared" si="26"/>
-        <v>1.262878852643214</v>
-      </c>
-      <c r="L65" s="20">
-        <f t="shared" si="26"/>
-        <v>-0.3536187596994495</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
+      <c r="B79" s="20">
+        <f>B64/B7</f>
+        <v>0.20735655750165349</v>
+      </c>
+      <c r="C79" s="20">
+        <f>C64/C7</f>
+        <v>9.2035971505810887E-2</v>
+      </c>
+      <c r="D79" s="20">
+        <f>D64/D7</f>
+        <v>-0.46613582271894538</v>
+      </c>
+      <c r="E79" s="20">
+        <f>E64/E7</f>
+        <v>-0.35057409793105471</v>
+      </c>
+      <c r="F79" s="20">
+        <f>F64/F7</f>
+        <v>-0.20102261425125806</v>
+      </c>
+      <c r="G79" s="20">
+        <f>G64/G7</f>
+        <v>0.25292531061148837</v>
+      </c>
+      <c r="H79" s="20">
+        <f>H64/H7</f>
+        <v>-0.17972151400376934</v>
+      </c>
+      <c r="I79" s="20">
+        <f>I64/I7</f>
+        <v>5.8618015065193763E-2</v>
+      </c>
+      <c r="J79" s="20">
+        <f>J64/J7</f>
+        <v>-0.85644909229749655</v>
+      </c>
+      <c r="K79" s="20">
+        <f>K64/K7</f>
+        <v>0.90670240372556909</v>
+      </c>
+      <c r="L79" s="20">
+        <f t="shared" ref="L79" si="33">L64/L7</f>
+        <v>-0.37433270745870745</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B66" s="20">
-        <f t="shared" ref="B66:L66" si="27">B51/B8</f>
-        <v>-0.72230333067463626</v>
-      </c>
-      <c r="C66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.43694498411908977</v>
-      </c>
-      <c r="D66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.43801200099236581</v>
-      </c>
-      <c r="E66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.34272631318403218</v>
-      </c>
-      <c r="F66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.1739477119884994</v>
-      </c>
-      <c r="G66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.40005517526981149</v>
-      </c>
-      <c r="H66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.25108163472415695</v>
-      </c>
-      <c r="I66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.74364194682175733</v>
-      </c>
-      <c r="J66" s="20">
-        <f t="shared" si="27"/>
-        <v>-1.1294690691957647</v>
-      </c>
-      <c r="K66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.50553610994822218</v>
-      </c>
-      <c r="L66" s="20">
-        <f t="shared" si="27"/>
-        <v>-0.36257578683663422</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
+      <c r="B80" s="20">
+        <f>B65/B8</f>
+        <v>-0.51941552379763434</v>
+      </c>
+      <c r="C80" s="20">
+        <f>C65/C8</f>
+        <v>-0.25833345359570858</v>
+      </c>
+      <c r="D80" s="20">
+        <f>D65/D8</f>
+        <v>-0.36536088140151385</v>
+      </c>
+      <c r="E80" s="20">
+        <f>E65/E8</f>
+        <v>-0.4002670607507971</v>
+      </c>
+      <c r="F80" s="20">
+        <f>F65/F8</f>
+        <v>-9.3941040952409433E-2</v>
+      </c>
+      <c r="G80" s="20">
+        <f>G65/G8</f>
+        <v>-0.41416759210471321</v>
+      </c>
+      <c r="H80" s="20">
+        <f>H65/H8</f>
+        <v>-4.9195445404302672E-2</v>
+      </c>
+      <c r="I80" s="20">
+        <f>I65/I8</f>
+        <v>-0.60684096994411174</v>
+      </c>
+      <c r="J80" s="20">
+        <f>J65/J8</f>
+        <v>-0.94310768747788964</v>
+      </c>
+      <c r="K80" s="20">
+        <f>K65/K8</f>
+        <v>-0.30010810903349022</v>
+      </c>
+      <c r="L80" s="20">
+        <f t="shared" ref="L80" si="34">L65/L8</f>
+        <v>-0.35867137454742232</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B67" s="20">
-        <f t="shared" ref="B67:L67" si="28">B52/B9</f>
-        <v>-0.18689605560268466</v>
-      </c>
-      <c r="C67" s="20">
-        <f t="shared" si="28"/>
-        <v>0.23200384771445831</v>
-      </c>
-      <c r="D67" s="20">
-        <f t="shared" si="28"/>
-        <v>-0.45707559395195935</v>
-      </c>
-      <c r="E67" s="20">
-        <f t="shared" si="28"/>
-        <v>-0.1316125461659908</v>
-      </c>
-      <c r="F67" s="20">
-        <f t="shared" si="28"/>
-        <v>8.7297267323386551E-2</v>
-      </c>
-      <c r="G67" s="20">
-        <f t="shared" si="28"/>
-        <v>1.1790469866163662</v>
-      </c>
-      <c r="H67" s="20">
-        <f t="shared" si="28"/>
-        <v>0.71825006720513229</v>
-      </c>
-      <c r="I67" s="20">
-        <f t="shared" si="28"/>
-        <v>-0.10598025212578521</v>
-      </c>
-      <c r="J67" s="20">
-        <f t="shared" si="28"/>
-        <v>5.1244327667423232E-3</v>
-      </c>
-      <c r="K67" s="20">
-        <f t="shared" si="28"/>
-        <v>1.0906916766567982E-2</v>
-      </c>
-      <c r="L67" s="20">
-        <f t="shared" si="28"/>
-        <v>0.14289146335466679</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A68" s="9" t="s">
+      <c r="B81" s="20">
+        <f>B66/B9</f>
+        <v>-6.9754971919038303E-3</v>
+      </c>
+      <c r="C81" s="20">
+        <f>C66/C9</f>
+        <v>0.53135804611129156</v>
+      </c>
+      <c r="D81" s="20">
+        <f>D66/D9</f>
+        <v>-0.27605254094313486</v>
+      </c>
+      <c r="E81" s="20">
+        <f>E66/E9</f>
+        <v>-4.8990888969699199E-2</v>
+      </c>
+      <c r="F81" s="20">
+        <f>F66/F9</f>
+        <v>4.7819672528707523E-2</v>
+      </c>
+      <c r="G81" s="20">
+        <f>G66/G9</f>
+        <v>1.2095739803644059</v>
+      </c>
+      <c r="H81" s="20">
+        <f>H66/H9</f>
+        <v>0.85650271330908578</v>
+      </c>
+      <c r="I81" s="20">
+        <f>I66/I9</f>
+        <v>0.10602632390056471</v>
+      </c>
+      <c r="J81" s="20">
+        <f>J66/J9</f>
+        <v>0.6042623826500183</v>
+      </c>
+      <c r="K81" s="20">
+        <f>K66/K9</f>
+        <v>3.0277631502766796E-2</v>
+      </c>
+      <c r="L81" s="20">
+        <f t="shared" ref="L81" si="35">L66/L9</f>
+        <v>0.16208368272682486</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="20">
-        <f t="shared" ref="B68:L68" si="29">B53/B10</f>
-        <v>0.26042688676326659</v>
-      </c>
-      <c r="C68" s="20">
-        <f t="shared" si="29"/>
-        <v>0.2241814645975522</v>
-      </c>
-      <c r="D68" s="20">
-        <f t="shared" si="29"/>
-        <v>0.1214795253801586</v>
-      </c>
-      <c r="E68" s="20">
-        <f t="shared" si="29"/>
-        <v>-0.4493847561804728</v>
-      </c>
-      <c r="F68" s="20">
-        <f t="shared" si="29"/>
-        <v>1.0340548271847039</v>
-      </c>
-      <c r="G68" s="20">
-        <f t="shared" si="29"/>
-        <v>-0.12100241726284328</v>
-      </c>
-      <c r="H68" s="20">
-        <f t="shared" si="29"/>
-        <v>0.5576989464099531</v>
-      </c>
-      <c r="I68" s="20">
-        <f t="shared" si="29"/>
-        <v>0.10047568306113158</v>
-      </c>
-      <c r="J68" s="20">
-        <f t="shared" si="29"/>
-        <v>-0.5325981378313267</v>
-      </c>
-      <c r="K68" s="20">
-        <f t="shared" si="29"/>
-        <v>1.0756940072604446</v>
-      </c>
-      <c r="L68" s="20">
-        <f t="shared" si="29"/>
-        <v>-6.3370340064001246E-2</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="9" t="s">
+      <c r="B82" s="20">
+        <f>B67/B10</f>
+        <v>0.23798106328920385</v>
+      </c>
+      <c r="C82" s="20">
+        <f>C67/C10</f>
+        <v>0.22937700998375887</v>
+      </c>
+      <c r="D82" s="20">
+        <f>D67/D10</f>
+        <v>0.17352797728642225</v>
+      </c>
+      <c r="E82" s="20">
+        <f>E67/E10</f>
+        <v>-0.46326391597238809</v>
+      </c>
+      <c r="F82" s="20">
+        <f>F67/F10</f>
+        <v>1.0704863440683352</v>
+      </c>
+      <c r="G82" s="20">
+        <f>G67/G10</f>
+        <v>-0.10985115235844975</v>
+      </c>
+      <c r="H82" s="20">
+        <f>H67/H10</f>
+        <v>0.64866470913576135</v>
+      </c>
+      <c r="I82" s="20">
+        <f>I67/I10</f>
+        <v>0.1251037943078645</v>
+      </c>
+      <c r="J82" s="20">
+        <f>J67/J10</f>
+        <v>9.390527573254237E-2</v>
+      </c>
+      <c r="K82" s="20">
+        <f>K67/K10</f>
+        <v>0.75260033723358044</v>
+      </c>
+      <c r="L82" s="20">
+        <f t="shared" ref="L82" si="36">L67/L10</f>
+        <v>-5.0288829066596777E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B69" s="20">
-        <f t="shared" ref="B69:L69" si="30">B54/B11</f>
-        <v>1.6622726562176839</v>
-      </c>
-      <c r="C69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.426072785639101</v>
-      </c>
-      <c r="D69" s="20">
-        <f t="shared" si="30"/>
-        <v>-0.18494341346955157</v>
-      </c>
-      <c r="E69" s="20">
-        <f t="shared" si="30"/>
-        <v>-0.27857485059578885</v>
-      </c>
-      <c r="F69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.70304655356014678</v>
-      </c>
-      <c r="G69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.47028553774803161</v>
-      </c>
-      <c r="H69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.3740707326586088</v>
-      </c>
-      <c r="I69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.22844085034675654</v>
-      </c>
-      <c r="J69" s="20">
-        <f t="shared" si="30"/>
-        <v>8.5999373819909564E-3</v>
-      </c>
-      <c r="K69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.30412566494872595</v>
-      </c>
-      <c r="L69" s="20">
-        <f t="shared" si="30"/>
-        <v>0.3704366021198206</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+      <c r="B83" s="20">
+        <f>B68/B11</f>
+        <v>2.479283171850962</v>
+      </c>
+      <c r="C83" s="20">
+        <f>C68/C11</f>
+        <v>0.79228913431197434</v>
+      </c>
+      <c r="D83" s="20">
+        <f>D68/D11</f>
+        <v>6.8663365396047574E-2</v>
+      </c>
+      <c r="E83" s="20">
+        <f>E68/E11</f>
+        <v>-8.2908599524955745E-2</v>
+      </c>
+      <c r="F83" s="20">
+        <f>F68/F11</f>
+        <v>0.84178347296859168</v>
+      </c>
+      <c r="G83" s="20">
+        <f>G68/G11</f>
+        <v>0.55919485302575833</v>
+      </c>
+      <c r="H83" s="20">
+        <f>H68/H11</f>
+        <v>0.39158214210068065</v>
+      </c>
+      <c r="I83" s="20">
+        <f>I68/I11</f>
+        <v>0.46148169101884917</v>
+      </c>
+      <c r="J83" s="20">
+        <f>J68/J11</f>
+        <v>1.6075665213866788</v>
+      </c>
+      <c r="K83" s="20">
+        <f>K68/K11</f>
+        <v>0.39737395802555153</v>
+      </c>
+      <c r="L83" s="20">
+        <f t="shared" ref="L83" si="37">L68/L11</f>
+        <v>0.42126648150065854</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="20">
-        <f t="shared" ref="B70:L70" si="31">B55/B12</f>
-        <v>-0.45168991306496792</v>
-      </c>
-      <c r="C70" s="20">
-        <f t="shared" si="31"/>
-        <v>-0.82811174444984426</v>
-      </c>
-      <c r="D70" s="20">
-        <f t="shared" si="31"/>
-        <v>-0.50860435989584973</v>
-      </c>
-      <c r="E70" s="20">
-        <f t="shared" si="31"/>
-        <v>-0.70440819876600413</v>
-      </c>
-      <c r="F70" s="20">
-        <f t="shared" si="31"/>
-        <v>2.9350402403754351E-2</v>
-      </c>
-      <c r="G70" s="20">
-        <f t="shared" si="31"/>
-        <v>0.65087628073518944</v>
-      </c>
-      <c r="H70" s="20">
-        <f t="shared" si="31"/>
-        <v>0.27423913664511018</v>
-      </c>
-      <c r="I70" s="20">
-        <f t="shared" si="31"/>
-        <v>-0.24755624570880211</v>
-      </c>
-      <c r="J70" s="20">
-        <f t="shared" si="31"/>
-        <v>-0.53845915612419404</v>
-      </c>
-      <c r="K70" s="20">
-        <f t="shared" si="31"/>
-        <v>0.3973406981247542</v>
-      </c>
-      <c r="L70" s="20">
-        <f t="shared" si="31"/>
-        <v>-8.3852716597154597E-2</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="B84" s="20">
+        <f>B69/B12</f>
+        <v>-0.50243914627657638</v>
+      </c>
+      <c r="C84" s="20">
+        <f>C69/C12</f>
+        <v>-0.71357702126275224</v>
+      </c>
+      <c r="D84" s="20">
+        <f>D69/D12</f>
+        <v>-0.4089563145149428</v>
+      </c>
+      <c r="E84" s="20">
+        <f>E69/E12</f>
+        <v>-0.56294884312583537</v>
+      </c>
+      <c r="F84" s="20">
+        <f>F69/F12</f>
+        <v>0.26375544367616566</v>
+      </c>
+      <c r="G84" s="20">
+        <f>G69/G12</f>
+        <v>0.73222847378533296</v>
+      </c>
+      <c r="H84" s="20">
+        <f>H69/H12</f>
+        <v>0.5100872442080332</v>
+      </c>
+      <c r="I84" s="20">
+        <f>I69/I12</f>
+        <v>-0.2177938305581745</v>
+      </c>
+      <c r="J84" s="20">
+        <f>J69/J12</f>
+        <v>2.216247862015567</v>
+      </c>
+      <c r="K84" s="20">
+        <f>K69/K12</f>
+        <v>0.2931444351039893</v>
+      </c>
+      <c r="L84" s="20">
+        <f t="shared" ref="L84" si="38">L69/L12</f>
+        <v>-4.3043877130955914E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B71" s="20">
-        <f t="shared" ref="B71:L71" si="32">B56/B13</f>
-        <v>-1.182576905497345</v>
-      </c>
-      <c r="C71" s="20">
-        <f t="shared" si="32"/>
-        <v>-1.1396992303260336</v>
-      </c>
-      <c r="D71" s="20">
-        <f t="shared" si="32"/>
-        <v>-1.0918532866395754</v>
-      </c>
-      <c r="E71" s="20">
-        <f t="shared" si="32"/>
-        <v>-1.1034927194832849</v>
-      </c>
-      <c r="F71" s="20">
-        <f t="shared" si="32"/>
-        <v>0.50699235278179766</v>
-      </c>
-      <c r="G71" s="20">
-        <f t="shared" si="32"/>
-        <v>-0.40361075843232536</v>
-      </c>
-      <c r="H71" s="20">
-        <f t="shared" si="32"/>
-        <v>-9.3678688380889288E-2</v>
-      </c>
-      <c r="I71" s="20">
-        <f t="shared" si="32"/>
-        <v>-0.50103882171247616</v>
-      </c>
-      <c r="J71" s="20">
-        <f t="shared" si="32"/>
-        <v>-2.3217596668171788E-3</v>
-      </c>
-      <c r="K71" s="20">
-        <f t="shared" si="32"/>
-        <v>7.3885186037299003E-2</v>
-      </c>
-      <c r="L71" s="20">
-        <f t="shared" si="32"/>
-        <v>-2.6462391131769656E-2</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
+      <c r="B85" s="20">
+        <f>B70/B13</f>
+        <v>-0.90490106859465025</v>
+      </c>
+      <c r="C85" s="20">
+        <f>C70/C13</f>
+        <v>-0.92256811270596673</v>
+      </c>
+      <c r="D85" s="20">
+        <f>D70/D13</f>
+        <v>-0.75892313423133029</v>
+      </c>
+      <c r="E85" s="20">
+        <f>E70/E13</f>
+        <v>-0.91091558012285767</v>
+      </c>
+      <c r="F85" s="20">
+        <f>F70/F13</f>
+        <v>1.217181115995414</v>
+      </c>
+      <c r="G85" s="20">
+        <f>G70/G13</f>
+        <v>0.29922007936259337</v>
+      </c>
+      <c r="H85" s="20">
+        <f>H70/H13</f>
+        <v>1.5077604269890261</v>
+      </c>
+      <c r="I85" s="20">
+        <f>I70/I13</f>
+        <v>2.4714161903922256</v>
+      </c>
+      <c r="J85" s="20">
+        <f>J70/J13</f>
+        <v>0.29518351121323028</v>
+      </c>
+      <c r="K85" s="20">
+        <f>K70/K13</f>
+        <v>-0.39950973186751643</v>
+      </c>
+      <c r="L85" s="20">
+        <f t="shared" ref="L85" si="39">L70/L13</f>
+        <v>0.27973275872692854</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="20">
-        <f t="shared" ref="B72:L72" si="33">B57/B14</f>
-        <v>0.18645696761377245</v>
-      </c>
-      <c r="C72" s="20">
-        <f t="shared" si="33"/>
-        <v>7.7122904638099019</v>
-      </c>
-      <c r="D72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.78609194059006304</v>
-      </c>
-      <c r="E72" s="20">
-        <f t="shared" si="33"/>
-        <v>-0.55458064032436427</v>
-      </c>
-      <c r="F72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.52560365111431828</v>
-      </c>
-      <c r="G72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.8887957693755183</v>
-      </c>
-      <c r="H72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.22395823145860028</v>
-      </c>
-      <c r="I72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.44152420713015411</v>
-      </c>
-      <c r="J72" s="20">
-        <f t="shared" si="33"/>
-        <v>5.7882074955825598E-2</v>
-      </c>
-      <c r="K72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.1408347895236825</v>
-      </c>
-      <c r="L72" s="20">
-        <f t="shared" si="33"/>
-        <v>0.18244937362885771</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
+      <c r="B86" s="20">
+        <f>B71/B14</f>
+        <v>-0.27820885235644477</v>
+      </c>
+      <c r="C86" s="20">
+        <f>C71/C14</f>
+        <v>6.4680787031532168</v>
+      </c>
+      <c r="D86" s="20">
+        <f>D71/D14</f>
+        <v>0.52659021067728273</v>
+      </c>
+      <c r="E86" s="20">
+        <f>E71/E14</f>
+        <v>-0.34817977123269084</v>
+      </c>
+      <c r="F86" s="20">
+        <f>F71/F14</f>
+        <v>0.5540001061488371</v>
+      </c>
+      <c r="G86" s="20">
+        <f>G71/G14</f>
+        <v>0.583547544135397</v>
+      </c>
+      <c r="H86" s="20">
+        <f>H71/H14</f>
+        <v>0.31384785765411394</v>
+      </c>
+      <c r="I86" s="20">
+        <f>I71/I14</f>
+        <v>0.33498346640358634</v>
+      </c>
+      <c r="J86" s="20">
+        <f>J71/J14</f>
+        <v>-0.41906183611884174</v>
+      </c>
+      <c r="K86" s="20">
+        <f>K71/K14</f>
+        <v>-0.1392377539821994</v>
+      </c>
+      <c r="L86" s="20">
+        <f t="shared" ref="L86" si="40">L71/L14</f>
+        <v>-5.726674739262929E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B73" s="20">
-        <f t="shared" ref="B73:L73" si="34">B58/B15</f>
-        <v>0.22104732942747804</v>
-      </c>
-      <c r="C73" s="20">
-        <f t="shared" si="34"/>
-        <v>-0.13259498292739336</v>
-      </c>
-      <c r="D73" s="20">
-        <f t="shared" si="34"/>
-        <v>-0.35386508149966189</v>
-      </c>
-      <c r="E73" s="20">
-        <f>E58/E15</f>
-        <v>-0.36213611745644908</v>
-      </c>
-      <c r="F73" s="20">
-        <f t="shared" si="34"/>
-        <v>0.14614775646615152</v>
-      </c>
-      <c r="G73" s="20">
-        <f t="shared" si="34"/>
-        <v>-6.2034998757330269E-2</v>
-      </c>
-      <c r="H73" s="20">
-        <f t="shared" si="34"/>
-        <v>0.36867951880703986</v>
-      </c>
-      <c r="I73" s="20">
-        <f t="shared" si="34"/>
-        <v>-8.0727883406192705E-2</v>
-      </c>
-      <c r="J73" s="20">
-        <f t="shared" si="34"/>
-        <v>-3.0750324179580759E-2</v>
-      </c>
-      <c r="K73" s="20">
-        <f t="shared" si="34"/>
-        <v>0.18136631586972998</v>
-      </c>
-      <c r="L73" s="20">
-        <f t="shared" si="34"/>
+      <c r="B87" s="20">
+        <f>B72/B15</f>
+        <v>0.18329745912149381</v>
+      </c>
+      <c r="C87" s="20">
+        <f>C72/C15</f>
+        <v>-0.1014918672577034</v>
+      </c>
+      <c r="D87" s="20">
+        <f>D72/D15</f>
+        <v>-0.37450236075189408</v>
+      </c>
+      <c r="E87" s="20">
+        <f>E72/E15</f>
+        <v>-0.35823180383159853</v>
+      </c>
+      <c r="F87" s="20">
+        <f>F72/F15</f>
+        <v>0.16533619034332442</v>
+      </c>
+      <c r="G87" s="20">
+        <f>G72/G15</f>
+        <v>-4.8957353203204212E-2</v>
+      </c>
+      <c r="H87" s="20">
+        <f>H72/H15</f>
+        <v>0.41942063748363367</v>
+      </c>
+      <c r="I87" s="20">
+        <f>I72/I15</f>
+        <v>-3.9738533544158239E-2</v>
+      </c>
+      <c r="J87" s="20">
+        <f>J72/J15</f>
+        <v>0.27441766627759928</v>
+      </c>
+      <c r="K87" s="20">
+        <f>K72/K15</f>
+        <v>-5.8176934531362953E-2</v>
+      </c>
+      <c r="L87" s="20">
+        <f t="shared" ref="L87" si="41">L72/L15</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B63:L73 N63">
+  <conditionalFormatting sqref="B77:L87 N77">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6006,7 +6699,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B48:L58">
+  <conditionalFormatting sqref="B62:L72">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>